<commit_message>
updated spredsheet with vacuous modifier
</commit_message>
<xml_diff>
--- a/The Lemon Taco spreadsheet edition.xlsx
+++ b/The Lemon Taco spreadsheet edition.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="386">
   <si>
     <t>name</t>
   </si>
@@ -1170,6 +1170,12 @@
   </si>
   <si>
     <t>adds 8(I think) modifiers to the tool</t>
+  </si>
+  <si>
+    <t>vacuous</t>
+  </si>
+  <si>
+    <t>hopper &amp; ender pearl</t>
   </si>
 </sst>
 </file>
@@ -5890,7 +5896,7 @@
   <dimension ref="A1:Q113"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A119" sqref="A119:XFD119"/>
@@ -11148,10 +11154,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11734,7 +11740,7 @@
         <v>450</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -11866,6 +11872,20 @@
         <v>36</v>
       </c>
       <c r="E67" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D68" s="1">
+        <v>1</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>373</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added crooked and smashing modifiers to spreadsheet
</commit_message>
<xml_diff>
--- a/The Lemon Taco spreadsheet edition.xlsx
+++ b/The Lemon Taco spreadsheet edition.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="390">
   <si>
     <t>name</t>
   </si>
@@ -1157,9 +1157,6 @@
     <t>obsidian &amp; ender pearl</t>
   </si>
   <si>
-    <t>stackable</t>
-  </si>
-  <si>
     <t>increases durability by 500 and increases mining level to 3 if the current level is lower than 3</t>
   </si>
   <si>
@@ -1176,6 +1173,21 @@
   </si>
   <si>
     <t>hopper &amp; ender pearl</t>
+  </si>
+  <si>
+    <t>usable</t>
+  </si>
+  <si>
+    <t>crooked</t>
+  </si>
+  <si>
+    <t>bone crook</t>
+  </si>
+  <si>
+    <t>diamond hammer</t>
+  </si>
+  <si>
+    <t>smashing</t>
   </si>
 </sst>
 </file>
@@ -5896,7 +5908,7 @@
   <dimension ref="A1:Q113"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A119" sqref="A119:XFD119"/>
@@ -11154,10 +11166,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11166,7 +11178,7 @@
     <col min="2" max="2" width="58" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -11579,10 +11591,10 @@
         <v>346</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -11641,7 +11653,7 @@
         <v>371</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>361</v>
@@ -11672,7 +11684,7 @@
         <v>85</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>85</v>
@@ -11790,7 +11802,7 @@
         <v>355</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>366</v>
@@ -11877,16 +11889,44 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>385</v>
       </c>
       <c r="D68" s="1">
         <v>1</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>373</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="D70" s="1">
+        <v>1</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add fruit ores to generation and update spreadsheet
</commit_message>
<xml_diff>
--- a/The Lemon Taco spreadsheet edition.xlsx
+++ b/The Lemon Taco spreadsheet edition.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="397">
   <si>
     <t>name</t>
   </si>
@@ -1188,6 +1188,27 @@
   </si>
   <si>
     <t>smashing</t>
+  </si>
+  <si>
+    <t>will set attacked enemies on fire, the level indicates the duration</t>
+  </si>
+  <si>
+    <t>gives attacked enemies a weakness effect, the level indicates the duration</t>
+  </si>
+  <si>
+    <t>gives attacked enemies a poison effect, the level indicates the duration</t>
+  </si>
+  <si>
+    <t>gives attacked enemies a slowness effect, the level indicates the duration</t>
+  </si>
+  <si>
+    <t>gives attacked enemies a wither effect, the level indicates the duration</t>
+  </si>
+  <si>
+    <t>rubracium dust</t>
+  </si>
+  <si>
+    <t>whetstone powder</t>
   </si>
 </sst>
 </file>
@@ -1254,7 +1275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1288,6 +1309,9 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -11169,13 +11193,13 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="51.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -11464,29 +11488,41 @@
       <c r="A31" s="1" t="s">
         <v>302</v>
       </c>
+      <c r="B31" s="1" t="s">
+        <v>390</v>
+      </c>
       <c r="C31" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>303</v>
       </c>
+      <c r="B32" s="1" t="s">
+        <v>391</v>
+      </c>
       <c r="C32" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>304</v>
       </c>
+      <c r="B33" s="1" t="s">
+        <v>392</v>
+      </c>
       <c r="C33" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>227</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>393</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>77</v>
@@ -11503,9 +11539,12 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>231</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>394</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>81</v>
@@ -11670,7 +11709,7 @@
         <v>348</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>50</v>
+        <v>395</v>
       </c>
       <c r="D53" s="1">
         <v>50</v>
@@ -11713,17 +11752,17 @@
         <v>375</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="16" t="s">
         <v>349</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="D56" s="1">
-        <v>1</v>
-      </c>
-      <c r="E56" s="1" t="s">
+      <c r="D56" s="16">
+        <v>1</v>
+      </c>
+      <c r="E56" s="16" t="s">
         <v>375</v>
       </c>
     </row>
@@ -11760,7 +11799,7 @@
         <v>352</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>52</v>
+        <v>396</v>
       </c>
       <c r="D59" s="1">
         <v>72</v>

</xml_diff>

<commit_message>
Fix for colorblind.json & misc wip stuff
</commit_message>
<xml_diff>
--- a/The Lemon Taco spreadsheet edition.xlsx
+++ b/The Lemon Taco spreadsheet edition.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="oregen" sheetId="1" r:id="rId1"/>
     <sheet name="toolmaterial stats" sheetId="2" r:id="rId2"/>
     <sheet name="lemonades" sheetId="3" r:id="rId3"/>
-    <sheet name="ore dictionary" sheetId="4" r:id="rId4"/>
-    <sheet name="explanation" sheetId="5" r:id="rId5"/>
+    <sheet name="explanation" sheetId="5" r:id="rId4"/>
+    <sheet name="ore dictionary" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="397">
   <si>
     <t>name</t>
   </si>
@@ -1142,9 +1142,6 @@
     <t>multiple</t>
   </si>
   <si>
-    <t>increases durability by 50%</t>
-  </si>
-  <si>
     <t>single</t>
   </si>
   <si>
@@ -1166,9 +1163,6 @@
     <t>items per modifier</t>
   </si>
   <si>
-    <t>adds 8(I think) modifiers to the tool</t>
-  </si>
-  <si>
     <t>vacuous</t>
   </si>
   <si>
@@ -1209,6 +1203,12 @@
   </si>
   <si>
     <t>whetstone powder</t>
+  </si>
+  <si>
+    <t>adds 5 modifiers to the tool</t>
+  </si>
+  <si>
+    <t>increases durability by 50% and increases mining level to 2 if the current level is lower than 2</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1310,8 +1310,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1929,11 +1932,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B97" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A104" sqref="A104:XFD104"/>
+      <selection pane="bottomRight" activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2067,6 +2070,9 @@
       <c r="M4" t="s">
         <v>246</v>
       </c>
+      <c r="N4" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2109,6 +2115,9 @@
       <c r="M5" t="s">
         <v>246</v>
       </c>
+      <c r="N5" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2151,6 +2160,9 @@
       <c r="M6" t="s">
         <v>246</v>
       </c>
+      <c r="N6" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2187,6 +2199,9 @@
       <c r="M7" t="s">
         <v>246</v>
       </c>
+      <c r="N7" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2229,6 +2244,9 @@
       <c r="M8" t="s">
         <v>246</v>
       </c>
+      <c r="N8" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2271,6 +2289,9 @@
       <c r="M9" t="s">
         <v>246</v>
       </c>
+      <c r="N9" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2313,6 +2334,9 @@
       <c r="M10" t="s">
         <v>246</v>
       </c>
+      <c r="N10" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2355,6 +2379,9 @@
       <c r="M11" t="s">
         <v>246</v>
       </c>
+      <c r="N11" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2391,6 +2418,9 @@
       <c r="M12" t="s">
         <v>246</v>
       </c>
+      <c r="N12" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2427,6 +2457,9 @@
       <c r="M13" t="s">
         <v>246</v>
       </c>
+      <c r="N13" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2466,6 +2499,9 @@
       <c r="M14" t="s">
         <v>246</v>
       </c>
+      <c r="N14" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2505,6 +2541,9 @@
       <c r="M15" t="s">
         <v>245</v>
       </c>
+      <c r="N15" t="s">
+        <v>246</v>
+      </c>
       <c r="O15" t="s">
         <v>288</v>
       </c>
@@ -2547,6 +2586,9 @@
       <c r="M16" t="s">
         <v>246</v>
       </c>
+      <c r="N16" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -2586,6 +2628,9 @@
       <c r="M17" t="s">
         <v>246</v>
       </c>
+      <c r="N17" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -2628,6 +2673,9 @@
       <c r="M18" t="s">
         <v>246</v>
       </c>
+      <c r="N18" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -2667,6 +2715,9 @@
       <c r="M19" t="s">
         <v>246</v>
       </c>
+      <c r="N19" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2706,6 +2757,9 @@
       <c r="M20" t="s">
         <v>246</v>
       </c>
+      <c r="N20" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -2745,6 +2799,9 @@
       <c r="M21" t="s">
         <v>246</v>
       </c>
+      <c r="N21" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2784,6 +2841,9 @@
       <c r="M22" t="s">
         <v>246</v>
       </c>
+      <c r="N22" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -2823,6 +2883,9 @@
       <c r="M23" t="s">
         <v>246</v>
       </c>
+      <c r="N23" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -2862,6 +2925,9 @@
       <c r="M24" t="s">
         <v>246</v>
       </c>
+      <c r="N24" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -2901,6 +2967,9 @@
       <c r="M25" t="s">
         <v>246</v>
       </c>
+      <c r="N25" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -2940,6 +3009,9 @@
       <c r="M26" t="s">
         <v>246</v>
       </c>
+      <c r="N26" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -2979,6 +3051,9 @@
       <c r="M27" t="s">
         <v>246</v>
       </c>
+      <c r="N27" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -3015,6 +3090,9 @@
       <c r="M28" t="s">
         <v>246</v>
       </c>
+      <c r="N28" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -3051,6 +3129,9 @@
       <c r="M29" t="s">
         <v>246</v>
       </c>
+      <c r="N29" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -3087,6 +3168,9 @@
       <c r="M30" t="s">
         <v>246</v>
       </c>
+      <c r="N30" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -3126,6 +3210,9 @@
       <c r="M31" t="s">
         <v>246</v>
       </c>
+      <c r="N31" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="32" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
@@ -3162,7 +3249,7 @@
       <c r="L32" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="M32" t="s">
+      <c r="M32" s="11" t="s">
         <v>246</v>
       </c>
       <c r="N32" s="11" t="s">
@@ -3172,7 +3259,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -3210,8 +3297,11 @@
       <c r="M33" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -3249,8 +3339,11 @@
       <c r="M34" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -3288,8 +3381,11 @@
       <c r="M35" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -3327,8 +3423,11 @@
       <c r="M36" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -3366,8 +3465,11 @@
       <c r="M37" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -3405,8 +3507,11 @@
       <c r="M38" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -3444,8 +3549,11 @@
       <c r="M39" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -3483,8 +3591,11 @@
       <c r="M40" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -3522,8 +3633,11 @@
       <c r="M41" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -3561,8 +3675,11 @@
       <c r="M42" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -3600,8 +3717,11 @@
       <c r="M43" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>76</v>
       </c>
@@ -3639,8 +3759,11 @@
       <c r="M44" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>77</v>
       </c>
@@ -3678,8 +3801,11 @@
       <c r="M45" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -3717,8 +3843,11 @@
       <c r="M46" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>83</v>
       </c>
@@ -3756,8 +3885,11 @@
       <c r="M47" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -3795,6 +3927,9 @@
       <c r="M48" t="s">
         <v>246</v>
       </c>
+      <c r="N48" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -3834,6 +3969,9 @@
       <c r="M49" t="s">
         <v>246</v>
       </c>
+      <c r="N49" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -3873,6 +4011,9 @@
       <c r="M50" t="s">
         <v>246</v>
       </c>
+      <c r="N50" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -3912,6 +4053,9 @@
       <c r="M51" t="s">
         <v>246</v>
       </c>
+      <c r="N51" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -4068,6 +4212,9 @@
       <c r="M55" t="s">
         <v>246</v>
       </c>
+      <c r="N55" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -4107,6 +4254,9 @@
       <c r="M56" t="s">
         <v>246</v>
       </c>
+      <c r="N56" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -4146,6 +4296,9 @@
       <c r="M57" t="s">
         <v>246</v>
       </c>
+      <c r="N57" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -5587,7 +5740,7 @@
         <v>3</v>
       </c>
       <c r="I95">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J95" t="s">
         <v>57</v>
@@ -5602,7 +5755,7 @@
         <v>246</v>
       </c>
       <c r="N95" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
@@ -5629,7 +5782,7 @@
         <v>3</v>
       </c>
       <c r="I96">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J96" t="s">
         <v>57</v>
@@ -5644,7 +5797,7 @@
         <v>246</v>
       </c>
       <c r="N96" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
@@ -5671,7 +5824,7 @@
         <v>3</v>
       </c>
       <c r="I97">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J97" t="s">
         <v>57</v>
@@ -5686,7 +5839,7 @@
         <v>246</v>
       </c>
       <c r="N97" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
@@ -5713,7 +5866,7 @@
         <v>3</v>
       </c>
       <c r="I98">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J98" t="s">
         <v>57</v>
@@ -5728,7 +5881,7 @@
         <v>246</v>
       </c>
       <c r="N98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -11076,11 +11229,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11123,51 +11276,51 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>140</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B8" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>141</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B9" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>142</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B10" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>143</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B11" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>144</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B12" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>287</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B13" t="s">
         <v>103</v>
       </c>
     </row>
@@ -11177,6 +11330,792 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E70"/>
+  <sheetViews>
+    <sheetView topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.7109375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="51.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>-1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>0</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>1</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>2</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>3</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>4</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>5</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>6</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>7</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>337</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>309</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>390</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>391</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>392</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>295</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="D49" s="16">
+        <v>1</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="D50" s="16">
+        <v>1</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="D51" s="16">
+        <v>1</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>371</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>395</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="D52" s="16">
+        <v>1</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>393</v>
+      </c>
+      <c r="D53" s="16">
+        <v>50</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="16">
+        <v>1</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D55" s="16">
+        <v>1</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="D56" s="17">
+        <v>1</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>363</v>
+      </c>
+      <c r="D57" s="16">
+        <v>1</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D58" s="16">
+        <v>450</v>
+      </c>
+      <c r="E58" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>394</v>
+      </c>
+      <c r="D59" s="16">
+        <v>72</v>
+      </c>
+      <c r="E59" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="D60" s="16">
+        <v>25</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="D61" s="16">
+        <v>1</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="D62" s="16">
+        <v>1</v>
+      </c>
+      <c r="E62" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="D63" s="16">
+        <v>1</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="D64" s="16">
+        <v>10</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="D65" s="16">
+        <v>1</v>
+      </c>
+      <c r="E65" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>369</v>
+      </c>
+      <c r="D66" s="16">
+        <v>4</v>
+      </c>
+      <c r="E66" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>370</v>
+      </c>
+      <c r="D67" s="16">
+        <v>36</v>
+      </c>
+      <c r="E67" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="D68" s="16">
+        <v>1</v>
+      </c>
+      <c r="E68" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>386</v>
+      </c>
+      <c r="D69" s="16">
+        <v>1</v>
+      </c>
+      <c r="E69" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="C70" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="D70" s="16">
+        <v>1</v>
+      </c>
+      <c r="E70" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -11186,790 +12125,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>-1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="D50" s="1">
-        <v>1</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="D51" s="1">
-        <v>1</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="D52" s="1">
-        <v>1</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="D53" s="1">
-        <v>50</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D54" s="1">
-        <v>1</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D55" s="1">
-        <v>1</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="16" t="s">
-        <v>349</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="D56" s="16">
-        <v>1</v>
-      </c>
-      <c r="E56" s="16" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="D57" s="1">
-        <v>1</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D58" s="1">
-        <v>450</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="D59" s="1">
-        <v>72</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="D60" s="1">
-        <v>25</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="D61" s="1">
-        <v>1</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="D62" s="1">
-        <v>1</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="D63" s="1">
-        <v>1</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="D64" s="1">
-        <v>10</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="D65" s="1">
-        <v>1</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="D66" s="1">
-        <v>4</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="D67" s="1">
-        <v>36</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="D68" s="1">
-        <v>1</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="D69" s="1">
-        <v>1</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="D70" s="1">
-        <v>1</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add bin folder which is nessacary for any modpack
</commit_message>
<xml_diff>
--- a/The Lemon Taco spreadsheet edition.xlsx
+++ b/The Lemon Taco spreadsheet edition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="oregen" sheetId="1" r:id="rId1"/>
@@ -14,11 +14,12 @@
     <sheet name="ore dictionary" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="399">
   <si>
     <t>name</t>
   </si>
@@ -1209,6 +1210,12 @@
   </si>
   <si>
     <t>increases durability by 50% and increases mining level to 2 if the current level is lower than 2</t>
+  </si>
+  <si>
+    <t>spooky</t>
+  </si>
+  <si>
+    <t>exhausting</t>
   </si>
 </sst>
 </file>
@@ -1321,7 +1328,333 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="73">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A15D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD4FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA9672"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FFD57B00"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFAFFDFF"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD4FAFC"/>
+          <bgColor rgb="FFD4FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A15D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD4FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAA9672"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FFD57B00"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFAFFDFF"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD4FAFC"/>
+          <bgColor rgb="FFD4FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1618,7 +1951,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Simple" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Simple" pivot="0" count="1">
-      <tableStyleElement type="secondRowStripe" dxfId="34"/>
+      <tableStyleElement type="secondRowStripe" dxfId="72"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1932,7 +2265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="F75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1941,20 +2274,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -5959,55 +6292,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O60:O91">
-    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="15" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="16" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="6" operator="equal">
       <formula>"rock"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="7" operator="equal">
       <formula>"gem"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="8" operator="equal">
       <formula>"metal, fantasy"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="9" operator="equal">
       <formula>"metal, nether"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="10" operator="equal">
       <formula>"metal, ender"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="11" operator="equal">
       <formula>"metal, precious"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="12" operator="equal">
       <formula>"metal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="13" operator="equal">
       <formula>"fruit"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="14" operator="equal">
       <formula>"utility"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O21:O22 M1:N1048576">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="3" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="4" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="1" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="2" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6082,34 +6415,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q113"/>
+  <dimension ref="A1:Q115"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A119" sqref="A119:XFD119"/>
+      <selection pane="bottomRight" activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="6.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.25" style="2" customWidth="1"/>
     <col min="10" max="10" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.375" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.25" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" customWidth="1"/>
-    <col min="17" max="17" width="63.28515625" customWidth="1"/>
+    <col min="17" max="17" width="63.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -10876,9 +11209,51 @@
         <v>245</v>
       </c>
     </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114" t="s">
+        <v>397</v>
+      </c>
+      <c r="E114" t="s">
+        <v>235</v>
+      </c>
+      <c r="M114" s="9">
+        <f t="shared" ref="M114:M115" si="5">C114*B114/2250+(C114-1)/2.33+0+0+F114/5+G114/9+H114/3-I114/200+J114/5.8-K114/50-L114/1000</f>
+        <v>-0.42918454935622319</v>
+      </c>
+      <c r="N114" t="s">
+        <v>245</v>
+      </c>
+      <c r="O114" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>28</v>
+      </c>
+      <c r="D115" t="s">
+        <v>398</v>
+      </c>
+      <c r="E115" t="s">
+        <v>235</v>
+      </c>
+      <c r="M115" s="9">
+        <f t="shared" si="5"/>
+        <v>-0.42918454935622319</v>
+      </c>
+      <c r="N115" t="s">
+        <v>245</v>
+      </c>
+      <c r="O115" t="s">
+        <v>245</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="L1:L6 L8:L63 L65:L1048576">
-    <cfRule type="dataBar" priority="80">
+  <conditionalFormatting sqref="L1:L6 L8:L63 L65:L113 L116:L1048576">
+    <cfRule type="dataBar" priority="140">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10891,8 +11266,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F88:F1048576 F1:F86">
-    <cfRule type="dataBar" priority="94">
+  <conditionalFormatting sqref="F88:F113 F1:F86 F116:F1048576">
+    <cfRule type="dataBar" priority="154">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10905,8 +11280,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H88:H1048576 H1:H86">
-    <cfRule type="dataBar" priority="98">
+  <conditionalFormatting sqref="H88:H113 H1:H86 H116:H1048576">
+    <cfRule type="dataBar" priority="158">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10919,8 +11294,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J88:J1048576 J1:J63 J65:J86">
-    <cfRule type="dataBar" priority="102">
+  <conditionalFormatting sqref="J88:J113 J1:J63 J65:J86 J116:J1048576">
+    <cfRule type="dataBar" priority="162">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10933,8 +11308,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G88:G1048576 G1:G86">
-    <cfRule type="dataBar" priority="107">
+  <conditionalFormatting sqref="G88:G113 G1:G86 G116:G1048576">
+    <cfRule type="dataBar" priority="167">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -10947,61 +11322,61 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+  <conditionalFormatting sqref="N1:N113 N116:N1048576">
+    <cfRule type="cellIs" dxfId="56" priority="81" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="82" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:P7 O8 Q8 O9:P1048576">
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
+  <conditionalFormatting sqref="O1:P7 O8 Q8 O9:P113 O116:P1048576">
+    <cfRule type="cellIs" dxfId="54" priority="79" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="80" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="dire">
+  <conditionalFormatting sqref="D1:D113 D116:D1048576">
+    <cfRule type="containsText" dxfId="52" priority="61" operator="containsText" text="dire">
       <formula>NOT(ISERROR(SEARCH("dire",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="skullfire">
+    <cfRule type="containsText" dxfId="51" priority="62" operator="containsText" text="skullfire">
       <formula>NOT(ISERROR(SEARCH("skullfire",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="cosmic">
+    <cfRule type="containsText" dxfId="50" priority="63" operator="containsText" text="cosmic">
       <formula>NOT(ISERROR(SEARCH("cosmic",D1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="70" operator="equal">
       <formula>"supermassive"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="reinforced">
+    <cfRule type="containsText" dxfId="48" priority="71" operator="containsText" text="reinforced">
       <formula>NOT(ISERROR(SEARCH("reinforced",D1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="72" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="stonebound">
+    <cfRule type="containsText" dxfId="46" priority="73" operator="containsText" text="stonebound">
       <formula>NOT(ISERROR(SEARCH("stonebound",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
+  <conditionalFormatting sqref="E1:E113 E116:E1048576">
+    <cfRule type="cellIs" dxfId="45" priority="74" operator="equal">
       <formula>"part builder, part cast"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="75" operator="equal">
       <formula>"dire crafting table"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="76" operator="equal">
       <formula>"part builder"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="77" operator="equal">
       <formula>"part cast"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C88:C1048576 C1:C86">
-    <cfRule type="dataBar" priority="8">
+  <conditionalFormatting sqref="C88:C113 C1:C86 C116:C1048576">
+    <cfRule type="dataBar" priority="68">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11013,12 +11388,12 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="69" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M88:M1048576 M1:M86">
-    <cfRule type="dataBar" priority="7">
+  <conditionalFormatting sqref="M88:M113 M1:M86 M116:M1048576">
+    <cfRule type="dataBar" priority="67">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11031,21 +11406,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+  <conditionalFormatting sqref="J1:J113 J116:J1048576">
+    <cfRule type="cellIs" dxfId="40" priority="65" operator="equal">
       <formula>1.2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+  <conditionalFormatting sqref="L1:L113 L116:L1048576">
+    <cfRule type="cellIs" dxfId="39" priority="64" operator="equal">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I84:I1048576 I1:I82">
-    <cfRule type="cellIs" dxfId="0" priority="201" operator="equal">
+  <conditionalFormatting sqref="I84:I113 I1:I82 I116:I1048576">
+    <cfRule type="cellIs" dxfId="38" priority="261" operator="equal">
       <formula>40</formula>
     </cfRule>
-    <cfRule type="dataBar" priority="202">
+    <cfRule type="dataBar" priority="262">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11058,8 +11433,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K84:K1048576 K1:K82">
-    <cfRule type="dataBar" priority="207">
+  <conditionalFormatting sqref="K84:K113 K1:K82 K116:K1048576">
+    <cfRule type="dataBar" priority="267">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11071,7 +11446,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="208">
+    <cfRule type="dataBar" priority="268">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11084,8 +11459,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B88:B1048576 B84:B86 B1:B82">
-    <cfRule type="dataBar" priority="213">
+  <conditionalFormatting sqref="B88:B113 B84:B86 B1:B82 B116:B1048576">
+    <cfRule type="dataBar" priority="273">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -11094,6 +11469,448 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{C6B9336F-76F8-422A-8114-E315282FDD2F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L114">
+    <cfRule type="dataBar" priority="51">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="2" tint="-0.499984740745262"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8475AB2E-3FC0-454F-AB54-FCCE3694268F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F114">
+    <cfRule type="dataBar" priority="52">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F32456CC-2488-4F95-ACC0-C5A236E7249D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H114">
+    <cfRule type="dataBar" priority="53">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3EED116B-D6ED-49BB-B65D-C1877FBA9B2C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J114">
+    <cfRule type="dataBar" priority="54">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{66C75076-9D21-42A1-9645-CC34C554AC9B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G114">
+    <cfRule type="dataBar" priority="55">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B7915F92-8E61-4158-A713-0651886A1FAD}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N114">
+    <cfRule type="cellIs" dxfId="37" priority="49" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="50" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O114:P114">
+    <cfRule type="cellIs" dxfId="35" priority="47" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="48" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D114">
+    <cfRule type="containsText" dxfId="33" priority="31" operator="containsText" text="dire">
+      <formula>NOT(ISERROR(SEARCH("dire",D114)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="skullfire">
+      <formula>NOT(ISERROR(SEARCH("skullfire",D114)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="cosmic">
+      <formula>NOT(ISERROR(SEARCH("cosmic",D114)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
+      <formula>"supermassive"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="40" operator="containsText" text="reinforced">
+      <formula>NOT(ISERROR(SEARCH("reinforced",D114)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="41" operator="equal">
+      <formula>"none"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="42" operator="containsText" text="stonebound">
+      <formula>NOT(ISERROR(SEARCH("stonebound",D114)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E114">
+    <cfRule type="cellIs" dxfId="26" priority="43" operator="equal">
+      <formula>"part builder, part cast"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="44" operator="equal">
+      <formula>"dire crafting table"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="45" operator="equal">
+      <formula>"part builder"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="46" operator="equal">
+      <formula>"part cast"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C114">
+    <cfRule type="dataBar" priority="37">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BB950044-A805-4F51-9435-2FB0007BE827}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="38" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M114">
+    <cfRule type="dataBar" priority="36">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF00B050"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6958E9BB-21F8-4B4E-B404-E193F043649A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J114">
+    <cfRule type="cellIs" dxfId="21" priority="35" operator="equal">
+      <formula>1.2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L114">
+    <cfRule type="cellIs" dxfId="20" priority="34" operator="equal">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I114">
+    <cfRule type="cellIs" dxfId="19" priority="56" operator="equal">
+      <formula>40</formula>
+    </cfRule>
+    <cfRule type="dataBar" priority="57">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B0FCAFD5-8860-4BA4-BD73-10B37415A488}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K114">
+    <cfRule type="dataBar" priority="58">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="7" tint="0.39997558519241921"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A951C96D-9A8C-4746-95CC-2144C0788FA0}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="dataBar" priority="59">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="7" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{17D643F4-9E29-42F7-8EAF-EAC6766DF215}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B114">
+    <cfRule type="dataBar" priority="60">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AFD0DD04-5B68-4BF6-A96D-61AE36FC19F0}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L115">
+    <cfRule type="dataBar" priority="21">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="2" tint="-0.499984740745262"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{994C38A8-D798-435B-80F1-4F44F88B04D3}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F115">
+    <cfRule type="dataBar" priority="22">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D62091D4-B2DA-462C-96E8-EA545ADD80CB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H115">
+    <cfRule type="dataBar" priority="23">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2A39306C-DCD4-425E-A242-6F3835177A2A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J115">
+    <cfRule type="dataBar" priority="24">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0992EF59-F171-447E-8E29-81B9E7D02E4A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G115">
+    <cfRule type="dataBar" priority="25">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{CA0621EA-877C-45E7-9303-88BABDFD61E9}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N115">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O115:P115">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D115">
+    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="dire">
+      <formula>NOT(ISERROR(SEARCH("dire",D115)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="skullfire">
+      <formula>NOT(ISERROR(SEARCH("skullfire",D115)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="cosmic">
+      <formula>NOT(ISERROR(SEARCH("cosmic",D115)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>"supermassive"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="reinforced">
+      <formula>NOT(ISERROR(SEARCH("reinforced",D115)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>"none"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="stonebound">
+      <formula>NOT(ISERROR(SEARCH("stonebound",D115)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E115">
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+      <formula>"part builder, part cast"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+      <formula>"dire crafting table"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
+      <formula>"part builder"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
+      <formula>"part cast"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C115">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EA8A0C45-9EC0-4854-BA8A-A807A6C10DB4}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M115">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF00B050"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A81131EA-8DD6-4B93-9762-C375747B647E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J115">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+      <formula>1.2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L115">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I115">
+    <cfRule type="cellIs" dxfId="0" priority="26" operator="equal">
+      <formula>40</formula>
+    </cfRule>
+    <cfRule type="dataBar" priority="27">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5B6FC56E-E658-4920-A5D2-A7F76A155DF0}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K115">
+    <cfRule type="dataBar" priority="28">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="7" tint="0.39997558519241921"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3116A062-2CAA-496C-B33E-E0E790A99AF8}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="dataBar" priority="29">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="7" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2DAA01CF-710B-4D0B-8E86-70D6104EDE3D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B115">
+    <cfRule type="dataBar" priority="30">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{17BC3CAB-B273-4DD6-9223-47AE88046362}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -11112,7 +11929,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>L1:L6 L8:L63 L65:L1048576</xm:sqref>
+          <xm:sqref>L1:L6 L8:L63 L65:L113 L116:L1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{820A0882-06F2-4B14-B9FB-9FA79AAF1278}">
@@ -11123,7 +11940,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F88:F1048576 F1:F86</xm:sqref>
+          <xm:sqref>F88:F113 F1:F86 F116:F1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{7873A36C-220C-4368-B136-3626FE516F15}">
@@ -11134,7 +11951,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H88:H1048576 H1:H86</xm:sqref>
+          <xm:sqref>H88:H113 H1:H86 H116:H1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{45F3CC12-6630-4EB2-B8A9-BFFADE8AA892}">
@@ -11145,7 +11962,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J88:J1048576 J1:J63 J65:J86</xm:sqref>
+          <xm:sqref>J88:J113 J1:J63 J65:J86 J116:J1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{37E283D3-36E4-4CAA-B5BB-FA7109F09680}">
@@ -11156,7 +11973,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G88:G1048576 G1:G86</xm:sqref>
+          <xm:sqref>G88:G113 G1:G86 G116:G1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4F4D3FE2-A666-405B-8F4F-F44A87CC1BA3}">
@@ -11166,7 +11983,7 @@
               <x14:negativeFillColor rgb="FFC00000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C88:C1048576 C1:C86</xm:sqref>
+          <xm:sqref>C88:C113 C1:C86 C116:C1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{93719E4B-6F9F-44BD-94E0-15B6B2AC544C}">
@@ -11178,7 +11995,7 @@
               <x14:negativeBorderColor rgb="FFFF0000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M88:M1048576 M1:M86</xm:sqref>
+          <xm:sqref>M88:M113 M1:M86 M116:M1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{07996D23-76D8-4AB7-A1B6-93F8F2B2D02D}">
@@ -11189,7 +12006,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I84:I1048576 I1:I82</xm:sqref>
+          <xm:sqref>I84:I113 I1:I82 I116:I1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5B934DB6-0548-4A24-B9F8-7FB71437DB09}">
@@ -11208,7 +12025,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>K84:K1048576 K1:K82</xm:sqref>
+          <xm:sqref>K84:K113 K1:K82 K116:K1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C6B9336F-76F8-422A-8114-E315282FDD2F}">
@@ -11219,7 +12036,243 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>B88:B1048576 B84:B86 B1:B82</xm:sqref>
+          <xm:sqref>B88:B113 B84:B86 B1:B82 B116:B1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8475AB2E-3FC0-454F-AB54-FCCE3694268F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L114</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F32456CC-2488-4F95-ACC0-C5A236E7249D}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F114</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3EED116B-D6ED-49BB-B65D-C1877FBA9B2C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H114</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{66C75076-9D21-42A1-9645-CC34C554AC9B}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J114</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B7915F92-8E61-4158-A713-0651886A1FAD}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G114</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BB950044-A805-4F51-9435-2FB0007BE827}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0" axisPosition="none">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFC00000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C114</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6958E9BB-21F8-4B4E-B404-E193F043649A}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarBorderColorSameAsPositive="0" axisPosition="none">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M114</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B0FCAFD5-8860-4BA4-BD73-10B37415A488}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I114</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A951C96D-9A8C-4746-95CC-2144C0788FA0}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <x14:cfRule type="dataBar" id="{17D643F4-9E29-42F7-8EAF-EAC6766DF215}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K114</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AFD0DD04-5B68-4BF6-A96D-61AE36FC19F0}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B114</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{994C38A8-D798-435B-80F1-4F44F88B04D3}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L115</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D62091D4-B2DA-462C-96E8-EA545ADD80CB}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F115</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2A39306C-DCD4-425E-A242-6F3835177A2A}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H115</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0992EF59-F171-447E-8E29-81B9E7D02E4A}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J115</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CA0621EA-877C-45E7-9303-88BABDFD61E9}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G115</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EA8A0C45-9EC0-4854-BA8A-A807A6C10DB4}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0" axisPosition="none">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFC00000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C115</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A81131EA-8DD6-4B93-9762-C375747B647E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarBorderColorSameAsPositive="0" axisPosition="none">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M115</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5B6FC56E-E658-4920-A5D2-A7F76A155DF0}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I115</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3116A062-2CAA-496C-B33E-E0E790A99AF8}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <x14:cfRule type="dataBar" id="{2DAA01CF-710B-4D0B-8E86-70D6104EDE3D}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K115</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{17BC3CAB-B273-4DD6-9223-47AE88046362}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B115</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -11238,8 +12291,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11337,17 +12390,17 @@
       <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.7109375" style="16" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="18.125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.75" style="16" customWidth="1"/>
+    <col min="3" max="3" width="51.125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.875" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>254</v>
       </c>
@@ -11355,7 +12408,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>-1</v>
       </c>
@@ -11363,7 +12416,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>0</v>
       </c>
@@ -11371,7 +12424,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>1</v>
       </c>
@@ -11379,7 +12432,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>2</v>
       </c>
@@ -11387,7 +12440,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>3</v>
       </c>
@@ -11395,7 +12448,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>4</v>
       </c>
@@ -11403,7 +12456,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>5</v>
       </c>
@@ -11411,7 +12464,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>6</v>
       </c>
@@ -11419,7 +12472,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>7</v>
       </c>
@@ -11427,7 +12480,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>156</v>
       </c>
@@ -11438,7 +12491,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>299</v>
       </c>
@@ -11449,7 +12502,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>300</v>
       </c>
@@ -11460,7 +12513,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>301</v>
       </c>
@@ -11471,7 +12524,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>212</v>
       </c>
@@ -11482,7 +12535,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>213</v>
       </c>
@@ -11493,7 +12546,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>215</v>
       </c>
@@ -11504,7 +12557,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>232</v>
       </c>
@@ -11515,7 +12568,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>315</v>
       </c>
@@ -11526,7 +12579,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>291</v>
       </c>
@@ -11537,7 +12590,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>297</v>
       </c>
@@ -11548,7 +12601,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>233</v>
       </c>
@@ -11559,7 +12612,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>305</v>
       </c>
@@ -11570,7 +12623,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>306</v>
       </c>
@@ -11581,7 +12634,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>307</v>
       </c>
@@ -11592,7 +12645,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>320</v>
       </c>
@@ -11603,7 +12656,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>319</v>
       </c>
@@ -11614,7 +12667,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>342</v>
       </c>
@@ -11625,7 +12678,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>302</v>
       </c>
@@ -11636,7 +12689,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>303</v>
       </c>
@@ -11647,7 +12700,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>304</v>
       </c>
@@ -11658,7 +12711,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>227</v>
       </c>
@@ -11669,7 +12722,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>229</v>
       </c>
@@ -11680,7 +12733,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>231</v>
       </c>
@@ -11691,7 +12744,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>239</v>
       </c>
@@ -11699,7 +12752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>294</v>
       </c>
@@ -11707,7 +12760,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>248</v>
       </c>
@@ -11715,7 +12768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>295</v>
       </c>
@@ -11723,7 +12776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>240</v>
       </c>
@@ -11731,12 +12784,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C42" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>251</v>
       </c>
@@ -11744,7 +12797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>241</v>
       </c>
@@ -11752,7 +12805,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>249</v>
       </c>
@@ -11760,7 +12813,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>345</v>
       </c>
@@ -11777,7 +12830,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>347</v>
       </c>
@@ -11794,7 +12847,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
         <v>347</v>
       </c>
@@ -11811,7 +12864,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>347</v>
       </c>
@@ -11828,7 +12881,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
         <v>371</v>
       </c>
@@ -11845,7 +12898,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
         <v>348</v>
       </c>
@@ -11859,7 +12912,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
         <v>85</v>
       </c>
@@ -11876,7 +12929,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
         <v>86</v>
       </c>
@@ -11907,7 +12960,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
         <v>350</v>
       </c>
@@ -11921,7 +12974,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
         <v>351</v>
       </c>
@@ -11935,7 +12988,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
         <v>352</v>
       </c>
@@ -11949,7 +13002,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
         <v>353</v>
       </c>
@@ -11963,7 +13016,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
         <v>354</v>
       </c>
@@ -11977,7 +13030,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
         <v>355</v>
       </c>
@@ -11994,7 +13047,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
         <v>301</v>
       </c>
@@ -12011,7 +13064,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
         <v>356</v>
       </c>
@@ -12025,7 +13078,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
         <v>376</v>
       </c>
@@ -12039,7 +13092,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
         <v>357</v>
       </c>
@@ -12053,7 +13106,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
         <v>23</v>
       </c>
@@ -12067,7 +13120,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
         <v>381</v>
       </c>
@@ -12081,7 +13134,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
         <v>387</v>
       </c>
@@ -12095,7 +13148,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
         <v>384</v>
       </c>

</xml_diff>

<commit_message>
part one of bad ores compatibility improvement
</commit_message>
<xml_diff>
--- a/The Lemon Taco spreadsheet edition.xlsx
+++ b/The Lemon Taco spreadsheet edition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="oregen" sheetId="1" r:id="rId1"/>
@@ -14,11 +14,12 @@
     <sheet name="ore dictionary" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="427">
   <si>
     <t>name</t>
   </si>
@@ -1263,6 +1264,42 @@
   </si>
   <si>
     <t>has a chance of crashing when used</t>
+  </si>
+  <si>
+    <t>shocking</t>
+  </si>
+  <si>
+    <t>murderous</t>
+  </si>
+  <si>
+    <t>superpositional</t>
+  </si>
+  <si>
+    <t>cleptomanic</t>
+  </si>
+  <si>
+    <t>scary</t>
+  </si>
+  <si>
+    <t>has a chance of killing the player when used</t>
+  </si>
+  <si>
+    <t>makes rocks rain from the sky when used</t>
+  </si>
+  <si>
+    <t>steals an item from the inventory when used</t>
+  </si>
+  <si>
+    <t>has a chance of jumpscaring the player when used</t>
+  </si>
+  <si>
+    <t>tools with this effect can not be picked up by players</t>
+  </si>
+  <si>
+    <t>quickly drains hunger when used</t>
+  </si>
+  <si>
+    <t>moves to a different spot in the inventory when used</t>
   </si>
 </sst>
 </file>
@@ -1375,47 +1412,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="77">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="73">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -2038,7 +2035,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Simple" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Simple" pivot="0" count="1">
-      <tableStyleElement type="secondRowStripe" dxfId="76"/>
+      <tableStyleElement type="secondRowStripe" dxfId="72"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2352,29 +2349,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L96" sqref="L96"/>
+      <selection pane="bottomRight" activeCell="N66" sqref="N66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -4515,6 +4513,9 @@
       <c r="M52" t="s">
         <v>246</v>
       </c>
+      <c r="N52" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -4554,6 +4555,9 @@
       <c r="M53" t="s">
         <v>246</v>
       </c>
+      <c r="N53" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -4592,6 +4596,9 @@
       </c>
       <c r="M54" t="s">
         <v>246</v>
+      </c>
+      <c r="N54" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -6379,55 +6386,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O60:O91">
-    <cfRule type="cellIs" dxfId="75" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="15" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="16" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="73" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="6" operator="equal">
       <formula>"rock"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="7" operator="equal">
       <formula>"gem"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="8" operator="equal">
       <formula>"metal, fantasy"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="9" operator="equal">
       <formula>"metal, nether"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="10" operator="equal">
       <formula>"metal, ender"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="11" operator="equal">
       <formula>"metal, precious"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="12" operator="equal">
       <formula>"metal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="13" operator="equal">
       <formula>"fruit"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="14" operator="equal">
       <formula>"utility"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O21:O22 M1:N1048576">
-    <cfRule type="cellIs" dxfId="64" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="3" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="4" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15">
-    <cfRule type="cellIs" dxfId="62" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="1" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="2" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6508,7 +6515,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomRight" activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10886,12 +10893,24 @@
       <c r="A96" t="s">
         <v>7</v>
       </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>-0.2</v>
+      </c>
       <c r="D96" t="s">
         <v>211</v>
       </c>
+      <c r="F96">
+        <v>4</v>
+      </c>
+      <c r="G96">
+        <v>6</v>
+      </c>
       <c r="M96" s="9">
         <f t="shared" si="4"/>
-        <v>-0.42918454935622319</v>
+        <v>0.95155631855030998</v>
       </c>
       <c r="N96" t="s">
         <v>245</v>
@@ -11052,7 +11071,7 @@
         <v>16</v>
       </c>
       <c r="D102" t="s">
-        <v>211</v>
+        <v>416</v>
       </c>
       <c r="M102" s="9">
         <f t="shared" si="4"/>
@@ -11070,7 +11089,7 @@
         <v>20</v>
       </c>
       <c r="D103" t="s">
-        <v>211</v>
+        <v>417</v>
       </c>
       <c r="M103" s="9">
         <f t="shared" si="4"/>
@@ -11108,9 +11127,6 @@
       <c r="A105" t="s">
         <v>22</v>
       </c>
-      <c r="D105" t="s">
-        <v>211</v>
-      </c>
       <c r="M105" s="9">
         <f t="shared" si="4"/>
         <v>-0.42918454935622319</v>
@@ -11132,6 +11148,9 @@
       <c r="C106">
         <v>0.7</v>
       </c>
+      <c r="D106" t="s">
+        <v>415</v>
+      </c>
       <c r="E106" t="s">
         <v>234</v>
       </c>
@@ -11159,9 +11178,6 @@
       <c r="A107" t="s">
         <v>104</v>
       </c>
-      <c r="D107" t="s">
-        <v>211</v>
-      </c>
       <c r="M107" s="9">
         <f t="shared" si="4"/>
         <v>-0.42918454935622319</v>
@@ -11178,7 +11194,7 @@
         <v>25</v>
       </c>
       <c r="D108" t="s">
-        <v>211</v>
+        <v>418</v>
       </c>
       <c r="M108" s="9">
         <f t="shared" si="4"/>
@@ -11195,9 +11211,6 @@
       <c r="A109" t="s">
         <v>26</v>
       </c>
-      <c r="D109" t="s">
-        <v>211</v>
-      </c>
       <c r="E109" t="s">
         <v>235</v>
       </c>
@@ -11352,7 +11365,7 @@
         <v>36</v>
       </c>
       <c r="D115" t="s">
-        <v>211</v>
+        <v>419</v>
       </c>
       <c r="E115" t="s">
         <v>235</v>
@@ -11482,55 +11495,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N118:N1048576 N1:N115">
-    <cfRule type="cellIs" dxfId="60" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="81" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="82" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:P7 O8 Q8 O118:P1048576 O9:P115">
-    <cfRule type="cellIs" dxfId="58" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="79" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="80" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D115 D118:D1048576">
-    <cfRule type="containsText" dxfId="56" priority="61" operator="containsText" text="dire">
+    <cfRule type="containsText" dxfId="52" priority="61" operator="containsText" text="dire">
       <formula>NOT(ISERROR(SEARCH("dire",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="62" operator="containsText" text="skullfire">
+    <cfRule type="containsText" dxfId="51" priority="62" operator="containsText" text="skullfire">
       <formula>NOT(ISERROR(SEARCH("skullfire",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="63" operator="containsText" text="cosmic">
+    <cfRule type="containsText" dxfId="50" priority="63" operator="containsText" text="cosmic">
       <formula>NOT(ISERROR(SEARCH("cosmic",D1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="70" operator="equal">
       <formula>"supermassive"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="71" operator="containsText" text="reinforced">
+    <cfRule type="containsText" dxfId="48" priority="71" operator="containsText" text="reinforced">
       <formula>NOT(ISERROR(SEARCH("reinforced",D1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="72" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="73" operator="containsText" text="stonebound">
+    <cfRule type="containsText" dxfId="46" priority="73" operator="containsText" text="stonebound">
       <formula>NOT(ISERROR(SEARCH("stonebound",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E115 E118:E1048576">
-    <cfRule type="cellIs" dxfId="49" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="74" operator="equal">
       <formula>"part builder, part cast"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="75" operator="equal">
       <formula>"dire crafting table"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="76" operator="equal">
       <formula>"part builder"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="77" operator="equal">
       <formula>"part cast"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11547,7 +11560,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="69" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="69" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11566,17 +11579,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J115 J118:J1048576">
-    <cfRule type="cellIs" dxfId="44" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="65" operator="equal">
       <formula>1.2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L115 L118:L1048576">
-    <cfRule type="cellIs" dxfId="43" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="64" operator="equal">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I86:I115 I1:I84 I118:I1048576">
-    <cfRule type="cellIs" dxfId="42" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="261" operator="equal">
       <formula>40</formula>
     </cfRule>
     <cfRule type="dataBar" priority="262">
@@ -11703,55 +11716,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N116">
-    <cfRule type="cellIs" dxfId="41" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="49" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="50" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O116:P116">
-    <cfRule type="cellIs" dxfId="39" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="47" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="48" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D116">
-    <cfRule type="containsText" dxfId="37" priority="31" operator="containsText" text="dire">
+    <cfRule type="containsText" dxfId="33" priority="31" operator="containsText" text="dire">
       <formula>NOT(ISERROR(SEARCH("dire",D116)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="32" operator="containsText" text="skullfire">
+    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="skullfire">
       <formula>NOT(ISERROR(SEARCH("skullfire",D116)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="cosmic">
+    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="cosmic">
       <formula>NOT(ISERROR(SEARCH("cosmic",D116)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
       <formula>"supermassive"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="40" operator="containsText" text="reinforced">
+    <cfRule type="containsText" dxfId="29" priority="40" operator="containsText" text="reinforced">
       <formula>NOT(ISERROR(SEARCH("reinforced",D116)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="41" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="42" operator="containsText" text="stonebound">
+    <cfRule type="containsText" dxfId="27" priority="42" operator="containsText" text="stonebound">
       <formula>NOT(ISERROR(SEARCH("stonebound",D116)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E116">
-    <cfRule type="cellIs" dxfId="30" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="43" operator="equal">
       <formula>"part builder, part cast"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="44" operator="equal">
       <formula>"dire crafting table"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="45" operator="equal">
       <formula>"part builder"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="46" operator="equal">
       <formula>"part cast"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11768,7 +11781,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="38" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="38" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11787,17 +11800,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J116">
-    <cfRule type="cellIs" dxfId="25" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="35" operator="equal">
       <formula>1.2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L116">
-    <cfRule type="cellIs" dxfId="24" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="34" operator="equal">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I116">
-    <cfRule type="cellIs" dxfId="23" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="56" operator="equal">
       <formula>40</formula>
     </cfRule>
     <cfRule type="dataBar" priority="57">
@@ -11924,55 +11937,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N117">
-    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O117:P117">
-    <cfRule type="cellIs" dxfId="20" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D117">
-    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="dire">
+    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="dire">
       <formula>NOT(ISERROR(SEARCH("dire",D117)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="skullfire">
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="skullfire">
       <formula>NOT(ISERROR(SEARCH("skullfire",D117)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="cosmic">
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="cosmic">
       <formula>NOT(ISERROR(SEARCH("cosmic",D117)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"supermassive"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="reinforced">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="reinforced">
       <formula>NOT(ISERROR(SEARCH("reinforced",D117)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="stonebound">
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="stonebound">
       <formula>NOT(ISERROR(SEARCH("stonebound",D117)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E117">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
       <formula>"part builder, part cast"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
       <formula>"dire crafting table"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
       <formula>"part builder"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
       <formula>"part cast"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11989,7 +12002,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12008,17 +12021,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J117">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>1.2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L117">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I117">
-    <cfRule type="cellIs" dxfId="4" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="26" operator="equal">
       <formula>40</formula>
     </cfRule>
     <cfRule type="dataBar" priority="27">
@@ -12543,10 +12556,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12970,216 +12983,162 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>416</v>
+      </c>
       <c r="B43" s="16" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>251</v>
+        <v>417</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>407</v>
+        <v>426</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>408</v>
-      </c>
       <c r="C45" s="16" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>249</v>
+        <v>415</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>418</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>422</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
-        <v>345</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>275</v>
-      </c>
       <c r="C49" s="16" t="s">
-        <v>346</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>380</v>
-      </c>
-      <c r="E49" s="16" t="s">
-        <v>383</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>347</v>
+        <v>251</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>372</v>
+        <v>407</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>358</v>
-      </c>
-      <c r="D50" s="16">
-        <v>1</v>
-      </c>
-      <c r="E50" s="16" t="s">
-        <v>374</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>347</v>
+        <v>241</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>372</v>
+        <v>408</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>359</v>
-      </c>
-      <c r="D51" s="16">
-        <v>1</v>
-      </c>
-      <c r="E51" s="16" t="s">
-        <v>374</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>347</v>
+        <v>249</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>372</v>
+        <v>409</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="D52" s="16">
-        <v>1</v>
-      </c>
-      <c r="E52" s="16" t="s">
-        <v>374</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
-        <v>371</v>
+        <v>419</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>395</v>
+        <v>423</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>361</v>
-      </c>
-      <c r="D53" s="16">
-        <v>1</v>
-      </c>
-      <c r="E53" s="16" t="s">
-        <v>374</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
-        <v>348</v>
+        <v>397</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>424</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>393</v>
-      </c>
-      <c r="D54" s="16">
-        <v>50</v>
-      </c>
-      <c r="E54" s="16" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>85</v>
+        <v>398</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>378</v>
+        <v>425</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="D55" s="16">
-        <v>1</v>
-      </c>
-      <c r="E55" s="16" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B56" s="16" t="s">
-        <v>396</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="D56" s="16">
-        <v>1</v>
-      </c>
-      <c r="E56" s="16" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="17" t="s">
-        <v>349</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>362</v>
-      </c>
-      <c r="D57" s="17">
-        <v>1</v>
-      </c>
-      <c r="E57" s="17" t="s">
-        <v>374</v>
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
-        <v>350</v>
+        <v>345</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>275</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>363</v>
-      </c>
-      <c r="D58" s="16">
-        <v>1</v>
+        <v>346</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>380</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>351</v>
+        <v>347</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>372</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>51</v>
+        <v>358</v>
       </c>
       <c r="D59" s="16">
-        <v>450</v>
+        <v>1</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>374</v>
@@ -13187,145 +13146,154 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
-        <v>352</v>
+        <v>347</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>372</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>394</v>
+        <v>359</v>
       </c>
       <c r="D60" s="16">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
-        <v>353</v>
+        <v>347</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>372</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D61" s="16">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>354</v>
+        <v>371</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>395</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D62" s="16">
         <v>1</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
-        <v>355</v>
-      </c>
-      <c r="B63" s="16" t="s">
-        <v>379</v>
+        <v>348</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>366</v>
+        <v>393</v>
       </c>
       <c r="D63" s="16">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
-        <v>301</v>
+        <v>85</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>367</v>
+        <v>85</v>
       </c>
       <c r="D64" s="16">
         <v>1</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
-        <v>356</v>
+        <v>86</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>396</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>368</v>
+        <v>86</v>
       </c>
       <c r="D65" s="16">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="16" t="s">
-        <v>376</v>
-      </c>
-      <c r="C66" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="D66" s="16">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="D66" s="17">
         <v>1</v>
       </c>
-      <c r="E66" s="16" t="s">
-        <v>373</v>
+      <c r="E66" s="17" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="D67" s="16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E67" s="16" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
-        <v>23</v>
+        <v>351</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>370</v>
+        <v>51</v>
       </c>
       <c r="D68" s="16">
-        <v>36</v>
+        <v>450</v>
       </c>
       <c r="E68" s="16" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
-        <v>381</v>
+        <v>352</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>382</v>
+        <v>394</v>
       </c>
       <c r="D69" s="16">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="E69" s="16" t="s">
         <v>373</v>
@@ -13333,29 +13301,161 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
-        <v>387</v>
+        <v>353</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>386</v>
+        <v>364</v>
       </c>
       <c r="D70" s="16">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
-        <v>384</v>
+        <v>354</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
       <c r="D71" s="16">
         <v>1</v>
       </c>
       <c r="E71" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="D72" s="16">
+        <v>1</v>
+      </c>
+      <c r="E72" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="C73" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="D73" s="16">
+        <v>1</v>
+      </c>
+      <c r="E73" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="C74" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="D74" s="16">
+        <v>10</v>
+      </c>
+      <c r="E74" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="C75" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="D75" s="16">
+        <v>1</v>
+      </c>
+      <c r="E75" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="C76" s="16" t="s">
+        <v>369</v>
+      </c>
+      <c r="D76" s="16">
+        <v>4</v>
+      </c>
+      <c r="E76" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" s="16" t="s">
+        <v>370</v>
+      </c>
+      <c r="D77" s="16">
+        <v>36</v>
+      </c>
+      <c r="E77" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="C78" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="D78" s="16">
+        <v>1</v>
+      </c>
+      <c r="E78" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="C79" s="16" t="s">
+        <v>386</v>
+      </c>
+      <c r="D79" s="16">
+        <v>1</v>
+      </c>
+      <c r="E79" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="C80" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="D80" s="16">
+        <v>1</v>
+      </c>
+      <c r="E80" s="16" t="s">
         <v>374</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Balanced (probably) orebush generation values
</commit_message>
<xml_diff>
--- a/The Lemon Taco spreadsheet edition.xlsx
+++ b/The Lemon Taco spreadsheet edition.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="432">
   <si>
     <t>name</t>
   </si>
@@ -1300,6 +1300,21 @@
   </si>
   <si>
     <t>moves to a different spot in the inventory when used</t>
+  </si>
+  <si>
+    <t>gen chance</t>
+  </si>
+  <si>
+    <t>growth chance</t>
+  </si>
+  <si>
+    <t>max y</t>
+  </si>
+  <si>
+    <t>vein size</t>
+  </si>
+  <si>
+    <t>oreberry bushes</t>
   </si>
 </sst>
 </file>
@@ -1412,7 +1427,253 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="73">
+  <dxfs count="148">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB59B79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF75"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD243"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA160E2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3B3B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF71FCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB59B79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF75"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD243"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA160E2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3B3B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF71FCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -2026,6 +2287,375 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB59B79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF75"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD243"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA160E2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3B3B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF71FCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB59B79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF75"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD243"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA160E2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3B3B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF71FCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB59B79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF75"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD243"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA160E2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3B3B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF71FCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
@@ -2035,7 +2665,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Simple" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Simple" pivot="0" count="1">
-      <tableStyleElement type="secondRowStripe" dxfId="72"/>
+      <tableStyleElement type="secondRowStripe" dxfId="147"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2347,13 +2977,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O98"/>
+  <dimension ref="A1:T98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N66" sqref="N66"/>
+      <selection pane="bottomRight" activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2373,9 +3003,14 @@
     <col min="13" max="13" width="6.875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2418,8 +3053,23 @@
       <c r="N1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>427</v>
+      </c>
+      <c r="R1" t="s">
+        <v>428</v>
+      </c>
+      <c r="S1" t="s">
+        <v>429</v>
+      </c>
+      <c r="T1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -2433,7 +3083,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -2447,7 +3097,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -2491,8 +3141,24 @@
       <c r="N4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <f>E4/10000</f>
+        <v>1.15E-2</v>
+      </c>
+      <c r="R4">
+        <f>E4/2500</f>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="S4">
+        <f>64*B4/100</f>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T4">
+        <f>ROUNDUP(E4/15,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2536,8 +3202,24 @@
       <c r="N5" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <f t="shared" ref="Q5:Q68" si="0">E5/10000</f>
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5:R68" si="1">E5/2500</f>
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="S5">
+        <f t="shared" ref="S5:S68" si="2">64*B5/100</f>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T5">
+        <f t="shared" ref="T5:T68" si="3">ROUNDUP(E5/15,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -2551,7 +3233,7 @@
         <v>39</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E57" si="0">AVERAGE(C6,D6)</f>
+        <f t="shared" ref="E6:E57" si="4">AVERAGE(C6,D6)</f>
         <v>37.5</v>
       </c>
       <c r="F6">
@@ -2581,8 +3263,24 @@
       <c r="N6" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>3.7499999999999999E-3</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="1"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -2596,7 +3294,7 @@
         <v>40</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="F7">
@@ -2620,8 +3318,24 @@
       <c r="N7" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="1"/>
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -2635,7 +3349,7 @@
         <v>46</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>39.5</v>
       </c>
       <c r="F8">
@@ -2665,8 +3379,24 @@
       <c r="N8" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>3.9500000000000004E-3</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="1"/>
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -2680,7 +3410,7 @@
         <v>45</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>41.5</v>
       </c>
       <c r="F9">
@@ -2710,8 +3440,24 @@
       <c r="N9" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>4.15E-3</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>1.66E-2</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -2725,7 +3471,7 @@
         <v>49</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>41.5</v>
       </c>
       <c r="F10">
@@ -2755,8 +3501,24 @@
       <c r="N10" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>4.15E-3</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="1"/>
+        <v>1.66E-2</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -2800,8 +3562,24 @@
       <c r="N11" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>1.44E-2</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2815,7 +3593,7 @@
         <v>46</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="F12">
@@ -2839,8 +3617,24 @@
       <c r="N12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="1"/>
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -2878,8 +3672,24 @@
       <c r="N13" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>9.5E-4</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>3.8E-3</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="2"/>
+        <v>33.28</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -2893,7 +3703,7 @@
         <v>11</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="F14">
@@ -2920,8 +3730,24 @@
       <c r="N14" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="1"/>
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="2"/>
+        <v>25.6</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -2965,8 +3791,24 @@
       <c r="O15" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="1"/>
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="2"/>
+        <v>25.6</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -2980,7 +3822,7 @@
         <v>36</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="F16">
@@ -3007,8 +3849,24 @@
       <c r="N16" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="1"/>
+        <v>1.24E-2</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="2"/>
+        <v>44.8</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -3022,7 +3880,7 @@
         <v>36</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="F17">
@@ -3049,8 +3907,24 @@
       <c r="N17" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <f t="shared" si="0"/>
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="1"/>
+        <v>1.24E-2</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="2"/>
+        <v>38.4</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -3064,7 +3938,7 @@
         <v>36</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="F18">
@@ -3094,8 +3968,24 @@
       <c r="N18" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <f t="shared" si="0"/>
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="1"/>
+        <v>1.24E-2</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="2"/>
+        <v>44.8</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>94</v>
       </c>
@@ -3109,7 +3999,7 @@
         <v>100</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>89.5</v>
       </c>
       <c r="F19">
@@ -3136,8 +4026,24 @@
       <c r="N19" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <f t="shared" si="0"/>
+        <v>8.9499999999999996E-3</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="1"/>
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>96</v>
       </c>
@@ -3151,7 +4057,7 @@
         <v>80</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
       <c r="F20">
@@ -3178,8 +4084,24 @@
       <c r="N20" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <f t="shared" si="0"/>
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="1"/>
+        <v>2.8400000000000002E-2</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="2"/>
+        <v>60.8</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>95</v>
       </c>
@@ -3193,7 +4115,7 @@
         <v>70</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="F21">
@@ -3220,8 +4142,24 @@
       <c r="N21" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <f t="shared" si="0"/>
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="1"/>
+        <v>2.4400000000000002E-2</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="2"/>
+        <v>52.48</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -3235,7 +4173,7 @@
         <v>46</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="F22">
@@ -3262,8 +4200,24 @@
       <c r="N22" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <f t="shared" si="0"/>
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="1"/>
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>115</v>
       </c>
@@ -3277,7 +4231,7 @@
         <v>31</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>28.5</v>
       </c>
       <c r="F23">
@@ -3304,8 +4258,24 @@
       <c r="N23" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <f t="shared" si="0"/>
+        <v>2.8500000000000001E-3</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="1"/>
+        <v>1.14E-2</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="2"/>
+        <v>43.52</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -3319,7 +4289,7 @@
         <v>33</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>29.5</v>
       </c>
       <c r="F24">
@@ -3346,8 +4316,24 @@
       <c r="N24" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <f t="shared" si="0"/>
+        <v>2.9499999999999999E-3</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="1"/>
+        <v>1.18E-2</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="2"/>
+        <v>60.8</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -3361,7 +4347,7 @@
         <v>20</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="F25">
@@ -3388,8 +4374,24 @@
       <c r="N25" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q25">
+        <f t="shared" si="0"/>
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="1"/>
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="2"/>
+        <v>38.4</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -3403,7 +4405,7 @@
         <v>12</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="F26">
@@ -3430,8 +4432,24 @@
       <c r="N26" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q26">
+        <f t="shared" si="0"/>
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="1"/>
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="2"/>
+        <v>28.8</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -3445,7 +4463,7 @@
         <v>3</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="F27">
@@ -3472,8 +4490,24 @@
       <c r="N27" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q27">
+        <f t="shared" si="0"/>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="1"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="2"/>
+        <v>22.4</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -3487,7 +4521,7 @@
         <v>40</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F28">
@@ -3511,8 +4545,24 @@
       <c r="N28" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q28">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="1"/>
+        <v>1.2E-2</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -3526,7 +4576,7 @@
         <v>30</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>22.5</v>
       </c>
       <c r="F29">
@@ -3550,8 +4600,24 @@
       <c r="N29" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q29">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999998E-3</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="1"/>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -3565,7 +4631,7 @@
         <v>20</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>17.5</v>
       </c>
       <c r="F30">
@@ -3589,8 +4655,24 @@
       <c r="N30" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q30">
+        <f t="shared" si="0"/>
+        <v>1.75E-3</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="2"/>
+        <v>60.8</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -3604,7 +4686,7 @@
         <v>16</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="F31">
@@ -3631,8 +4713,24 @@
       <c r="N31" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <f t="shared" si="0"/>
+        <v>1.4E-3</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="1"/>
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="2"/>
+        <v>58.88</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>278</v>
       </c>
@@ -3646,7 +4744,7 @@
         <v>14</v>
       </c>
       <c r="E32" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="F32" s="11">
@@ -3676,8 +4774,24 @@
       <c r="O32" s="11" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q32">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="1"/>
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="2"/>
+        <v>54.4</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -3691,7 +4805,7 @@
         <v>12</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="F33">
@@ -3718,8 +4832,24 @@
       <c r="N33" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q33">
+        <f t="shared" si="0"/>
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="1"/>
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="2"/>
+        <v>52.48</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -3733,7 +4863,7 @@
         <v>7</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>5.5</v>
       </c>
       <c r="F34">
@@ -3760,8 +4890,24 @@
       <c r="N34" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q34">
+        <f t="shared" si="0"/>
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="1"/>
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="2"/>
+        <v>44.8</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -3775,7 +4921,7 @@
         <v>4</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="F35">
@@ -3802,8 +4948,24 @@
       <c r="N35" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q35">
+        <f t="shared" si="0"/>
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="1"/>
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="2"/>
+        <v>38.4</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -3817,7 +4979,7 @@
         <v>2</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.5</v>
       </c>
       <c r="F36">
@@ -3844,8 +5006,24 @@
       <c r="N36" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q36">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="1"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -3859,7 +5037,7 @@
         <v>3</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="F37">
@@ -3886,8 +5064,24 @@
       <c r="N37" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q37">
+        <f t="shared" si="0"/>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="1"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="2"/>
+        <v>25.6</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -3901,7 +5095,7 @@
         <v>2</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F38">
@@ -3928,8 +5122,24 @@
       <c r="N38" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q38">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="2"/>
+        <v>21.12</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -3943,7 +5153,7 @@
         <v>2</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F39">
@@ -3970,8 +5180,24 @@
       <c r="N39" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q39">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="2"/>
+        <v>21.12</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -3985,7 +5211,7 @@
         <v>73</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>63.5</v>
       </c>
       <c r="F40">
@@ -4012,8 +5238,24 @@
       <c r="N40" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q40">
+        <f t="shared" si="0"/>
+        <v>6.3499999999999997E-3</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="1"/>
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="S40">
+        <f>120*B40/100</f>
+        <v>84</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -4027,7 +5269,7 @@
         <v>63</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>52.5</v>
       </c>
       <c r="F41">
@@ -4054,8 +5296,24 @@
       <c r="N41" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q41">
+        <f t="shared" si="0"/>
+        <v>5.2500000000000003E-3</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="1"/>
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="S41">
+        <f t="shared" ref="S41:S51" si="5">120*B41/100</f>
+        <v>132</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -4069,7 +5327,7 @@
         <v>46</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="F42">
@@ -4096,8 +5354,24 @@
       <c r="N42" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q42">
+        <f t="shared" si="0"/>
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="1"/>
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="5"/>
+        <v>132</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -4111,7 +5385,7 @@
         <v>50</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="F43">
@@ -4138,8 +5412,24 @@
       <c r="N43" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q43">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="5"/>
+        <v>132</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>76</v>
       </c>
@@ -4153,7 +5443,7 @@
         <v>21</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="F44">
@@ -4180,8 +5470,24 @@
       <c r="N44" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q44">
+        <f t="shared" si="0"/>
+        <v>1.9E-3</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="5"/>
+        <v>132</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>77</v>
       </c>
@@ -4195,7 +5501,7 @@
         <v>17</v>
       </c>
       <c r="E45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>14.5</v>
       </c>
       <c r="F45">
@@ -4222,8 +5528,24 @@
       <c r="N45" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q45">
+        <f t="shared" si="0"/>
+        <v>1.4499999999999999E-3</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="1"/>
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="5"/>
+        <v>132</v>
+      </c>
+      <c r="T45">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -4237,7 +5559,7 @@
         <v>13</v>
       </c>
       <c r="E46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="F46">
@@ -4264,8 +5586,24 @@
       <c r="N46" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q46">
+        <f t="shared" si="0"/>
+        <v>1E-3</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="5"/>
+        <v>132</v>
+      </c>
+      <c r="T46">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>83</v>
       </c>
@@ -4306,8 +5644,24 @@
       <c r="N47" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q47">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="1"/>
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="5"/>
+        <v>132</v>
+      </c>
+      <c r="T47">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -4321,7 +5675,7 @@
         <v>7</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="F48">
@@ -4348,8 +5702,24 @@
       <c r="N48" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q48">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="1"/>
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="5"/>
+        <v>132</v>
+      </c>
+      <c r="T48">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>82</v>
       </c>
@@ -4390,8 +5760,24 @@
       <c r="N49" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q49">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="1"/>
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="5"/>
+        <v>132</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>80</v>
       </c>
@@ -4405,7 +5791,7 @@
         <v>6</v>
       </c>
       <c r="E50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="F50">
@@ -4432,8 +5818,24 @@
       <c r="N50" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q50">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="1"/>
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="T50">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>81</v>
       </c>
@@ -4447,7 +5849,7 @@
         <v>2</v>
       </c>
       <c r="E51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F51">
@@ -4474,8 +5876,24 @@
       <c r="N51" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q51">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="T51">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>124</v>
       </c>
@@ -4489,7 +5907,7 @@
         <v>40</v>
       </c>
       <c r="E52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>34.5</v>
       </c>
       <c r="F52">
@@ -4516,8 +5934,24 @@
       <c r="N52" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q52">
+        <f t="shared" si="0"/>
+        <v>3.4499999999999999E-3</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="1"/>
+        <v>1.38E-2</v>
+      </c>
+      <c r="S52">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T52">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>125</v>
       </c>
@@ -4531,7 +5965,7 @@
         <v>27</v>
       </c>
       <c r="E53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="F53">
@@ -4558,8 +5992,24 @@
       <c r="N53" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q53">
+        <f t="shared" si="0"/>
+        <v>2.3E-3</v>
+      </c>
+      <c r="R53">
+        <f t="shared" si="1"/>
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="S53">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T53">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>126</v>
       </c>
@@ -4573,7 +6023,7 @@
         <v>13</v>
       </c>
       <c r="E54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="F54">
@@ -4600,8 +6050,24 @@
       <c r="N54" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q54">
+        <f t="shared" si="0"/>
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="1"/>
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T54">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>87</v>
       </c>
@@ -4642,8 +6108,24 @@
       <c r="N55" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q55">
+        <f t="shared" si="0"/>
+        <v>1.65E-3</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="1"/>
+        <v>6.6E-3</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="2"/>
+        <v>57.6</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -4657,7 +6139,7 @@
         <v>12</v>
       </c>
       <c r="E56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="F56">
@@ -4684,8 +6166,24 @@
       <c r="N56" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q56">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="R56">
+        <f t="shared" si="1"/>
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="S56">
+        <f t="shared" si="2"/>
+        <v>21.12</v>
+      </c>
+      <c r="T56">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>86</v>
       </c>
@@ -4699,7 +6197,7 @@
         <v>5</v>
       </c>
       <c r="E57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
       <c r="F57">
@@ -4726,8 +6224,24 @@
       <c r="N57" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q57">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R57">
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S57">
+        <f t="shared" si="2"/>
+        <v>60.8</v>
+      </c>
+      <c r="T57">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -4759,8 +6273,24 @@
       <c r="M58" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q58">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R58">
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S58">
+        <f t="shared" si="2"/>
+        <v>25.6</v>
+      </c>
+      <c r="T58">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -4774,7 +6304,7 @@
         <v>3</v>
       </c>
       <c r="E59">
-        <f t="shared" ref="E59:E77" si="1">AVERAGE(C59,D59)</f>
+        <f t="shared" ref="E59:E77" si="6">AVERAGE(C59,D59)</f>
         <v>2.5</v>
       </c>
       <c r="F59">
@@ -4792,8 +6322,24 @@
       <c r="M59" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q59">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R59">
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S59">
+        <f t="shared" si="2"/>
+        <v>23.04</v>
+      </c>
+      <c r="T59">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>262</v>
       </c>
@@ -4807,7 +6353,7 @@
         <v>3</v>
       </c>
       <c r="E60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F60">
@@ -4831,8 +6377,24 @@
       <c r="O60" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q60">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="2"/>
+        <v>51.2</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -4846,7 +6408,7 @@
         <v>3</v>
       </c>
       <c r="E61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F61">
@@ -4870,8 +6432,24 @@
       <c r="O61" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q61">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S61">
+        <f t="shared" si="2"/>
+        <v>37.119999999999997</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>15</v>
       </c>
@@ -4885,7 +6463,7 @@
         <v>3</v>
       </c>
       <c r="E62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F62">
@@ -4903,8 +6481,24 @@
       <c r="M62" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q62">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S62">
+        <f t="shared" si="2"/>
+        <v>38.4</v>
+      </c>
+      <c r="T62">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -4918,7 +6512,7 @@
         <v>3</v>
       </c>
       <c r="E63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F63">
@@ -4936,8 +6530,24 @@
       <c r="M63" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q63">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R63">
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S63">
+        <f t="shared" si="2"/>
+        <v>50.56</v>
+      </c>
+      <c r="T63">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -4951,7 +6561,7 @@
         <v>3</v>
       </c>
       <c r="E64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F64">
@@ -4975,8 +6585,24 @@
       <c r="O64" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q64">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R64">
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S64">
+        <f t="shared" si="2"/>
+        <v>32.64</v>
+      </c>
+      <c r="T64">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>22</v>
       </c>
@@ -4990,7 +6616,7 @@
         <v>3</v>
       </c>
       <c r="E65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F65">
@@ -5014,8 +6640,24 @@
       <c r="O65" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q65">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R65">
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S65">
+        <f t="shared" si="2"/>
+        <v>42.88</v>
+      </c>
+      <c r="T65">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>104</v>
       </c>
@@ -5029,7 +6671,7 @@
         <v>3</v>
       </c>
       <c r="E66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F66">
@@ -5053,8 +6695,24 @@
       <c r="M66" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q66">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R66">
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S66">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T66">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>25</v>
       </c>
@@ -5068,7 +6726,7 @@
         <v>3</v>
       </c>
       <c r="E67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F67">
@@ -5092,8 +6750,24 @@
       <c r="O67" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q67">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R67">
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S67">
+        <f t="shared" si="2"/>
+        <v>33.92</v>
+      </c>
+      <c r="T67">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>28</v>
       </c>
@@ -5107,7 +6781,7 @@
         <v>84</v>
       </c>
       <c r="E68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>76</v>
       </c>
       <c r="F68">
@@ -5131,8 +6805,24 @@
       <c r="M68" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q68">
+        <f t="shared" si="0"/>
+        <v>7.6E-3</v>
+      </c>
+      <c r="R68">
+        <f t="shared" si="1"/>
+        <v>3.04E-2</v>
+      </c>
+      <c r="S68">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T68">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>33</v>
       </c>
@@ -5146,7 +6836,7 @@
         <v>3</v>
       </c>
       <c r="E69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F69">
@@ -5170,8 +6860,24 @@
       <c r="O69" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q69">
+        <f t="shared" ref="Q69:Q98" si="7">E69/10000</f>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R69">
+        <f t="shared" ref="R69:R98" si="8">E69/2500</f>
+        <v>1E-3</v>
+      </c>
+      <c r="S69">
+        <f t="shared" ref="S69:S98" si="9">64*B69/100</f>
+        <v>62.08</v>
+      </c>
+      <c r="T69">
+        <f t="shared" ref="T69:T98" si="10">ROUNDUP(E69/15,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>36</v>
       </c>
@@ -5185,7 +6891,7 @@
         <v>3</v>
       </c>
       <c r="E70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F70">
@@ -5203,8 +6909,24 @@
       <c r="M70" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q70">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R70">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S70">
+        <f t="shared" si="9"/>
+        <v>26.24</v>
+      </c>
+      <c r="T70">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -5218,7 +6940,7 @@
         <v>3</v>
       </c>
       <c r="E71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F71">
@@ -5242,8 +6964,24 @@
       <c r="O71" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q71">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R71">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S71">
+        <f t="shared" si="9"/>
+        <v>55.04</v>
+      </c>
+      <c r="T71">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>21</v>
       </c>
@@ -5257,7 +6995,7 @@
         <v>84</v>
       </c>
       <c r="E72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>76</v>
       </c>
       <c r="F72">
@@ -5281,8 +7019,24 @@
       <c r="M72" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q72">
+        <f t="shared" si="7"/>
+        <v>7.6E-3</v>
+      </c>
+      <c r="R72">
+        <f t="shared" si="8"/>
+        <v>3.04E-2</v>
+      </c>
+      <c r="S72">
+        <f t="shared" si="9"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T72">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>24</v>
       </c>
@@ -5296,7 +7050,7 @@
         <v>2</v>
       </c>
       <c r="E73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="F73">
@@ -5320,8 +7074,24 @@
       <c r="M73" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q73">
+        <f t="shared" si="7"/>
+        <v>1E-4</v>
+      </c>
+      <c r="R73">
+        <f t="shared" si="8"/>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="S73">
+        <f t="shared" si="9"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T73">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>29</v>
       </c>
@@ -5335,7 +7105,7 @@
         <v>3</v>
       </c>
       <c r="E74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F74">
@@ -5365,8 +7135,24 @@
       <c r="O74" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q74">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R74">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S74">
+        <f t="shared" si="9"/>
+        <v>46.08</v>
+      </c>
+      <c r="T74">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>30</v>
       </c>
@@ -5380,7 +7166,7 @@
         <v>84</v>
       </c>
       <c r="E75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>76</v>
       </c>
       <c r="F75">
@@ -5404,8 +7190,24 @@
       <c r="M75" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q75">
+        <f t="shared" si="7"/>
+        <v>7.6E-3</v>
+      </c>
+      <c r="R75">
+        <f t="shared" si="8"/>
+        <v>3.04E-2</v>
+      </c>
+      <c r="S75">
+        <f t="shared" si="9"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T75">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>35</v>
       </c>
@@ -5419,7 +7221,7 @@
         <v>3</v>
       </c>
       <c r="E76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="F76">
@@ -5443,8 +7245,24 @@
       <c r="M76" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q76">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R76">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S76">
+        <f t="shared" si="9"/>
+        <v>19.2</v>
+      </c>
+      <c r="T76">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>37</v>
       </c>
@@ -5458,7 +7276,7 @@
         <v>38</v>
       </c>
       <c r="E77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="F77">
@@ -5488,8 +7306,24 @@
       <c r="O77" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q77">
+        <f t="shared" si="7"/>
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="R77">
+        <f t="shared" si="8"/>
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="S77">
+        <f t="shared" si="9"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T77">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>3</v>
       </c>
@@ -5503,7 +7337,7 @@
         <v>36</v>
       </c>
       <c r="E78">
-        <f t="shared" ref="E78:E87" si="2">AVERAGE(C78,D78)</f>
+        <f t="shared" ref="E78:E87" si="11">AVERAGE(C78,D78)</f>
         <v>31.5</v>
       </c>
       <c r="F78">
@@ -5530,8 +7364,24 @@
       <c r="O78" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q78">
+        <f t="shared" si="7"/>
+        <v>3.15E-3</v>
+      </c>
+      <c r="R78">
+        <f t="shared" si="8"/>
+        <v>1.26E-2</v>
+      </c>
+      <c r="S78">
+        <f t="shared" si="9"/>
+        <v>45.44</v>
+      </c>
+      <c r="T78">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>9</v>
       </c>
@@ -5545,7 +7395,7 @@
         <v>72</v>
       </c>
       <c r="E79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>62.5</v>
       </c>
       <c r="F79">
@@ -5563,8 +7413,24 @@
       <c r="M79" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q79">
+        <f t="shared" si="7"/>
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="R79">
+        <f t="shared" si="8"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S79">
+        <f t="shared" si="9"/>
+        <v>62.08</v>
+      </c>
+      <c r="T79">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -5578,7 +7444,7 @@
         <v>3</v>
       </c>
       <c r="E80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>2.5</v>
       </c>
       <c r="F80">
@@ -5602,8 +7468,24 @@
       <c r="M80" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q80">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R80">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S80">
+        <f t="shared" si="9"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T80">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>12</v>
       </c>
@@ -5617,7 +7499,7 @@
         <v>3</v>
       </c>
       <c r="E81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>2.5</v>
       </c>
       <c r="F81">
@@ -5641,8 +7523,24 @@
       <c r="O81" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q81">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R81">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S81">
+        <f t="shared" si="9"/>
+        <v>50.56</v>
+      </c>
+      <c r="T81">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>27</v>
       </c>
@@ -5656,7 +7554,7 @@
         <v>3</v>
       </c>
       <c r="E82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>2.5</v>
       </c>
       <c r="F82">
@@ -5674,8 +7572,24 @@
       <c r="M82" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q82">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R82">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S82">
+        <f t="shared" si="9"/>
+        <v>62.08</v>
+      </c>
+      <c r="T82">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>5</v>
       </c>
@@ -5689,7 +7603,7 @@
         <v>3</v>
       </c>
       <c r="E83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>2.5</v>
       </c>
       <c r="F83">
@@ -5707,8 +7621,24 @@
       <c r="M83" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q83">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R83">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S83">
+        <f t="shared" si="9"/>
+        <v>53.76</v>
+      </c>
+      <c r="T83">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>13</v>
       </c>
@@ -5722,7 +7652,7 @@
         <v>1</v>
       </c>
       <c r="E84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="F84">
@@ -5740,8 +7670,24 @@
       <c r="M84" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q84">
+        <f t="shared" si="7"/>
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="R84">
+        <f t="shared" si="8"/>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="S84">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="T84">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>17</v>
       </c>
@@ -5755,7 +7701,7 @@
         <v>3</v>
       </c>
       <c r="E85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>2.5</v>
       </c>
       <c r="F85">
@@ -5779,8 +7725,24 @@
       <c r="M85" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q85">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R85">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S85">
+        <f t="shared" si="9"/>
+        <v>56.32</v>
+      </c>
+      <c r="T85">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>26</v>
       </c>
@@ -5794,7 +7756,7 @@
         <v>3</v>
       </c>
       <c r="E86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>2.5</v>
       </c>
       <c r="F86">
@@ -5818,8 +7780,24 @@
       <c r="O86" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q86">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R86">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S86">
+        <f t="shared" si="9"/>
+        <v>28.8</v>
+      </c>
+      <c r="T86">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>18</v>
       </c>
@@ -5833,7 +7811,7 @@
         <v>3</v>
       </c>
       <c r="E87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>2.5</v>
       </c>
       <c r="F87">
@@ -5851,8 +7829,24 @@
       <c r="M87" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q87">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R87">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S87">
+        <f t="shared" si="9"/>
+        <v>22.4</v>
+      </c>
+      <c r="T87">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>4</v>
       </c>
@@ -5866,7 +7860,7 @@
         <v>3</v>
       </c>
       <c r="E88">
-        <f t="shared" ref="E88:E94" si="3">AVERAGE(C88,D88)</f>
+        <f t="shared" ref="E88:E94" si="12">AVERAGE(C88,D88)</f>
         <v>2.5</v>
       </c>
       <c r="F88">
@@ -5896,8 +7890,24 @@
       <c r="O88" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q88">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R88">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S88">
+        <f t="shared" si="9"/>
+        <v>40.96</v>
+      </c>
+      <c r="T88">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -5911,7 +7921,7 @@
         <v>3</v>
       </c>
       <c r="E89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>2.5</v>
       </c>
       <c r="F89">
@@ -5935,8 +7945,24 @@
       <c r="M89" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q89">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R89">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S89">
+        <f t="shared" si="9"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="T89">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>11</v>
       </c>
@@ -5950,7 +7976,7 @@
         <v>3</v>
       </c>
       <c r="E90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>2.5</v>
       </c>
       <c r="F90">
@@ -5980,8 +8006,24 @@
       <c r="O90" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q90">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R90">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S90">
+        <f t="shared" si="9"/>
+        <v>26.88</v>
+      </c>
+      <c r="T90">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>23</v>
       </c>
@@ -5995,7 +8037,7 @@
         <v>3</v>
       </c>
       <c r="E91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>2.5</v>
       </c>
       <c r="F91">
@@ -6025,8 +8067,24 @@
       <c r="O91" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q91">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R91">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S91">
+        <f t="shared" si="9"/>
+        <v>62.08</v>
+      </c>
+      <c r="T91">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>32</v>
       </c>
@@ -6040,7 +8098,7 @@
         <v>12</v>
       </c>
       <c r="E92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="F92">
@@ -6064,8 +8122,24 @@
       <c r="M92" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q92">
+        <f t="shared" si="7"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="R92">
+        <f t="shared" si="8"/>
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="S92">
+        <f t="shared" si="9"/>
+        <v>21.12</v>
+      </c>
+      <c r="T92">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>31</v>
       </c>
@@ -6079,7 +8153,7 @@
         <v>3</v>
       </c>
       <c r="E93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>2.5</v>
       </c>
       <c r="F93">
@@ -6103,8 +8177,24 @@
       <c r="M93" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q93">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R93">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S93">
+        <f t="shared" si="9"/>
+        <v>40.32</v>
+      </c>
+      <c r="T93">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>34</v>
       </c>
@@ -6118,7 +8208,7 @@
         <v>3</v>
       </c>
       <c r="E94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>2.5</v>
       </c>
       <c r="F94">
@@ -6142,8 +8232,24 @@
       <c r="M94" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q94">
+        <f t="shared" si="7"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="R94">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+      <c r="S94">
+        <f t="shared" si="9"/>
+        <v>19.2</v>
+      </c>
+      <c r="T94">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>53</v>
       </c>
@@ -6184,8 +8290,24 @@
       <c r="N95" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q95">
+        <f t="shared" si="7"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="R95">
+        <f t="shared" si="8"/>
+        <v>2.8E-3</v>
+      </c>
+      <c r="S95">
+        <f t="shared" si="9"/>
+        <v>14.08</v>
+      </c>
+      <c r="T95">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>54</v>
       </c>
@@ -6226,8 +8348,24 @@
       <c r="N96" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q96">
+        <f t="shared" si="7"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="R96">
+        <f t="shared" si="8"/>
+        <v>2.8E-3</v>
+      </c>
+      <c r="S96">
+        <f t="shared" si="9"/>
+        <v>14.08</v>
+      </c>
+      <c r="T96">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>55</v>
       </c>
@@ -6268,8 +8406,24 @@
       <c r="N97" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q97">
+        <f t="shared" si="7"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="R97">
+        <f t="shared" si="8"/>
+        <v>2.8E-3</v>
+      </c>
+      <c r="S97">
+        <f t="shared" si="9"/>
+        <v>14.08</v>
+      </c>
+      <c r="T97">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>56</v>
       </c>
@@ -6309,6 +8463,22 @@
       </c>
       <c r="N98" t="s">
         <v>246</v>
+      </c>
+      <c r="Q98">
+        <f t="shared" si="7"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="R98">
+        <f t="shared" si="8"/>
+        <v>2.8E-3</v>
+      </c>
+      <c r="S98">
+        <f t="shared" si="9"/>
+        <v>14.08</v>
+      </c>
+      <c r="T98">
+        <f t="shared" si="10"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6316,7 +8486,7 @@
     <sortCondition ref="J55:J91"/>
   </sortState>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="dataBar" priority="22">
+    <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6330,7 +8500,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="dataBar" priority="21">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6344,7 +8514,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="dataBar" priority="20">
+    <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6358,7 +8528,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:E1048576">
-    <cfRule type="dataBar" priority="19">
+    <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6372,7 +8542,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="dataBar" priority="18">
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6385,57 +8555,113 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O60:O91">
-    <cfRule type="cellIs" dxfId="71" priority="15" operator="equal">
+  <conditionalFormatting sqref="O60:P91">
+    <cfRule type="cellIs" dxfId="29" priority="19" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="20" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="69" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
       <formula>"rock"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
       <formula>"gem"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
       <formula>"metal, fantasy"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
       <formula>"metal, nether"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
       <formula>"metal, ender"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
       <formula>"metal, precious"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
       <formula>"metal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="17" operator="equal">
       <formula>"fruit"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
       <formula>"utility"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O21:O22 M1:N1048576">
-    <cfRule type="cellIs" dxfId="60" priority="3" operator="equal">
+  <conditionalFormatting sqref="O21:P22 M1:N1048576">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O15">
-    <cfRule type="cellIs" dxfId="58" priority="1" operator="equal">
+  <conditionalFormatting sqref="O15:P15">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q1:Q1048576">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="3" tint="0.39997558519241921"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C0F29000-9DBB-4CFA-9FFA-431FE5752635}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R1:R1048576">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{05F4DFCA-44C5-4E84-B907-41DC2EDE51F4}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S1:S1048576">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D10E24FC-244D-44C3-8E58-FCFB7F300932}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T1:T1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5FE04BEE-81D7-4E6A-98E3-9FD0333BAF97}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6500,6 +8726,50 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C0F29000-9DBB-4CFA-9FFA-431FE5752635}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>Q1:Q1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{05F4DFCA-44C5-4E84-B907-41DC2EDE51F4}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>R1:R1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D10E24FC-244D-44C3-8E58-FCFB7F300932}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>S1:S1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5FE04BEE-81D7-4E6A-98E3-9FD0333BAF97}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>T1:T1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -11495,55 +13765,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N118:N1048576 N1:N115">
-    <cfRule type="cellIs" dxfId="56" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="81" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="82" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:P7 O8 Q8 O118:P1048576 O9:P115">
-    <cfRule type="cellIs" dxfId="54" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="79" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="80" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D115 D118:D1048576">
-    <cfRule type="containsText" dxfId="52" priority="61" operator="containsText" text="dire">
+    <cfRule type="containsText" dxfId="82" priority="61" operator="containsText" text="dire">
       <formula>NOT(ISERROR(SEARCH("dire",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="62" operator="containsText" text="skullfire">
+    <cfRule type="containsText" dxfId="81" priority="62" operator="containsText" text="skullfire">
       <formula>NOT(ISERROR(SEARCH("skullfire",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="63" operator="containsText" text="cosmic">
+    <cfRule type="containsText" dxfId="80" priority="63" operator="containsText" text="cosmic">
       <formula>NOT(ISERROR(SEARCH("cosmic",D1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="70" operator="equal">
       <formula>"supermassive"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="71" operator="containsText" text="reinforced">
+    <cfRule type="containsText" dxfId="78" priority="71" operator="containsText" text="reinforced">
       <formula>NOT(ISERROR(SEARCH("reinforced",D1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="72" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="73" operator="containsText" text="stonebound">
+    <cfRule type="containsText" dxfId="76" priority="73" operator="containsText" text="stonebound">
       <formula>NOT(ISERROR(SEARCH("stonebound",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E115 E118:E1048576">
-    <cfRule type="cellIs" dxfId="45" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="74" operator="equal">
       <formula>"part builder, part cast"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="75" operator="equal">
       <formula>"dire crafting table"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="76" operator="equal">
       <formula>"part builder"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="77" operator="equal">
       <formula>"part cast"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11560,7 +13830,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="69" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="69" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11579,17 +13849,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J115 J118:J1048576">
-    <cfRule type="cellIs" dxfId="40" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="65" operator="equal">
       <formula>1.2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L115 L118:L1048576">
-    <cfRule type="cellIs" dxfId="39" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="64" operator="equal">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I86:I115 I1:I84 I118:I1048576">
-    <cfRule type="cellIs" dxfId="38" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="261" operator="equal">
       <formula>40</formula>
     </cfRule>
     <cfRule type="dataBar" priority="262">
@@ -11716,55 +13986,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N116">
-    <cfRule type="cellIs" dxfId="37" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="49" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="50" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O116:P116">
-    <cfRule type="cellIs" dxfId="35" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="47" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="48" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D116">
-    <cfRule type="containsText" dxfId="33" priority="31" operator="containsText" text="dire">
+    <cfRule type="containsText" dxfId="63" priority="31" operator="containsText" text="dire">
       <formula>NOT(ISERROR(SEARCH("dire",D116)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="skullfire">
+    <cfRule type="containsText" dxfId="62" priority="32" operator="containsText" text="skullfire">
       <formula>NOT(ISERROR(SEARCH("skullfire",D116)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="cosmic">
+    <cfRule type="containsText" dxfId="61" priority="33" operator="containsText" text="cosmic">
       <formula>NOT(ISERROR(SEARCH("cosmic",D116)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="39" operator="equal">
       <formula>"supermassive"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="40" operator="containsText" text="reinforced">
+    <cfRule type="containsText" dxfId="59" priority="40" operator="containsText" text="reinforced">
       <formula>NOT(ISERROR(SEARCH("reinforced",D116)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="41" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="42" operator="containsText" text="stonebound">
+    <cfRule type="containsText" dxfId="57" priority="42" operator="containsText" text="stonebound">
       <formula>NOT(ISERROR(SEARCH("stonebound",D116)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E116">
-    <cfRule type="cellIs" dxfId="26" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="43" operator="equal">
       <formula>"part builder, part cast"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="44" operator="equal">
       <formula>"dire crafting table"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="45" operator="equal">
       <formula>"part builder"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="46" operator="equal">
       <formula>"part cast"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11781,7 +14051,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="38" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="38" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11800,17 +14070,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J116">
-    <cfRule type="cellIs" dxfId="21" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="35" operator="equal">
       <formula>1.2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L116">
-    <cfRule type="cellIs" dxfId="20" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="34" operator="equal">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I116">
-    <cfRule type="cellIs" dxfId="19" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="56" operator="equal">
       <formula>40</formula>
     </cfRule>
     <cfRule type="dataBar" priority="57">
@@ -11937,55 +14207,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N117">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="19" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="20" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O117:P117">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="17" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="18" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D117">
-    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="dire">
+    <cfRule type="containsText" dxfId="44" priority="1" operator="containsText" text="dire">
       <formula>NOT(ISERROR(SEARCH("dire",D117)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="skullfire">
+    <cfRule type="containsText" dxfId="43" priority="2" operator="containsText" text="skullfire">
       <formula>NOT(ISERROR(SEARCH("skullfire",D117)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="cosmic">
+    <cfRule type="containsText" dxfId="42" priority="3" operator="containsText" text="cosmic">
       <formula>NOT(ISERROR(SEARCH("cosmic",D117)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="9" operator="equal">
       <formula>"supermassive"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="reinforced">
+    <cfRule type="containsText" dxfId="40" priority="10" operator="containsText" text="reinforced">
       <formula>NOT(ISERROR(SEARCH("reinforced",D117)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="11" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="stonebound">
+    <cfRule type="containsText" dxfId="38" priority="12" operator="containsText" text="stonebound">
       <formula>NOT(ISERROR(SEARCH("stonebound",D117)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E117">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="13" operator="equal">
       <formula>"part builder, part cast"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="14" operator="equal">
       <formula>"dire crafting table"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="15" operator="equal">
       <formula>"part builder"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="16" operator="equal">
       <formula>"part cast"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12002,7 +14272,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="8" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12021,17 +14291,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J117">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="5" operator="equal">
       <formula>1.2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L117">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="4" operator="equal">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I117">
-    <cfRule type="cellIs" dxfId="0" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
       <formula>40</formula>
     </cfRule>
     <cfRule type="dataBar" priority="27">
@@ -12558,7 +14828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Make erebus ores look umbery
</commit_message>
<xml_diff>
--- a/The Lemon Taco spreadsheet edition.xlsx
+++ b/The Lemon Taco spreadsheet edition.xlsx
@@ -2980,10 +2980,10 @@
   <dimension ref="A1:T98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O46" sqref="O46"/>
+      <selection pane="bottomRight" activeCell="V43" sqref="V43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3006,7 +3006,7 @@
     <col min="16" max="16" width="13.25" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.25" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3142,16 +3142,16 @@
         <v>246</v>
       </c>
       <c r="Q4">
-        <f>E4/10000</f>
-        <v>1.15E-2</v>
+        <f t="shared" ref="Q4:Q18" si="0">E4/5000</f>
+        <v>2.3E-2</v>
       </c>
       <c r="R4">
-        <f>E4/2500</f>
-        <v>4.5999999999999999E-2</v>
+        <f t="shared" ref="R4:R67" si="1">Q4*4</f>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="S4">
-        <f>64*B4/100</f>
-        <v>70.400000000000006</v>
+        <f>ROUND(64*B4/100,0)</f>
+        <v>70</v>
       </c>
       <c r="T4">
         <f>ROUNDUP(E4/15,0)</f>
@@ -3203,16 +3203,16 @@
         <v>246</v>
       </c>
       <c r="Q5">
-        <f t="shared" ref="Q5:Q68" si="0">E5/10000</f>
-        <v>3.8999999999999998E-3</v>
+        <f t="shared" si="0"/>
+        <v>7.7999999999999996E-3</v>
       </c>
       <c r="R5">
-        <f t="shared" ref="R5:R68" si="1">E5/2500</f>
-        <v>1.5599999999999999E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.1199999999999999E-2</v>
       </c>
       <c r="S5">
-        <f t="shared" ref="S5:S68" si="2">64*B5/100</f>
-        <v>70.400000000000006</v>
+        <f t="shared" ref="S5:S68" si="2">ROUND(64*B5/100,0)</f>
+        <v>70</v>
       </c>
       <c r="T5">
         <f t="shared" ref="T5:T68" si="3">ROUNDUP(E5/15,0)</f>
@@ -3265,15 +3265,15 @@
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>3.7499999999999999E-3</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="R6">
         <f t="shared" si="1"/>
-        <v>1.4999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="S6">
         <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T6">
         <f t="shared" si="3"/>
@@ -3320,15 +3320,15 @@
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>3.2000000000000002E-3</v>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="R7">
         <f t="shared" si="1"/>
-        <v>1.2800000000000001E-2</v>
+        <v>2.5600000000000001E-2</v>
       </c>
       <c r="S7">
         <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T7">
         <f t="shared" si="3"/>
@@ -3381,15 +3381,15 @@
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>3.9500000000000004E-3</v>
+        <v>7.9000000000000008E-3</v>
       </c>
       <c r="R8">
         <f t="shared" si="1"/>
-        <v>1.5800000000000002E-2</v>
+        <v>3.1600000000000003E-2</v>
       </c>
       <c r="S8">
         <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T8">
         <f t="shared" si="3"/>
@@ -3442,15 +3442,15 @@
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
-        <v>4.15E-3</v>
+        <v>8.3000000000000001E-3</v>
       </c>
       <c r="R9">
         <f t="shared" si="1"/>
-        <v>1.66E-2</v>
+        <v>3.32E-2</v>
       </c>
       <c r="S9">
         <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T9">
         <f t="shared" si="3"/>
@@ -3503,15 +3503,15 @@
       </c>
       <c r="Q10">
         <f t="shared" si="0"/>
-        <v>4.15E-3</v>
+        <v>8.3000000000000001E-3</v>
       </c>
       <c r="R10">
         <f t="shared" si="1"/>
-        <v>1.66E-2</v>
+        <v>3.32E-2</v>
       </c>
       <c r="S10">
         <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T10">
         <f t="shared" si="3"/>
@@ -3564,15 +3564,15 @@
       </c>
       <c r="Q11">
         <f t="shared" si="0"/>
-        <v>3.5999999999999999E-3</v>
+        <v>7.1999999999999998E-3</v>
       </c>
       <c r="R11">
         <f t="shared" si="1"/>
-        <v>1.44E-2</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="S11">
         <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T11">
         <f t="shared" si="3"/>
@@ -3619,15 +3619,15 @@
       </c>
       <c r="Q12">
         <f t="shared" si="0"/>
-        <v>4.1999999999999997E-3</v>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="R12">
         <f t="shared" si="1"/>
-        <v>1.6799999999999999E-2</v>
+        <v>3.3599999999999998E-2</v>
       </c>
       <c r="S12">
         <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T12">
         <f t="shared" si="3"/>
@@ -3674,15 +3674,15 @@
       </c>
       <c r="Q13">
         <f t="shared" si="0"/>
-        <v>9.5E-4</v>
+        <v>1.9E-3</v>
       </c>
       <c r="R13">
         <f t="shared" si="1"/>
-        <v>3.8E-3</v>
+        <v>7.6E-3</v>
       </c>
       <c r="S13">
         <f t="shared" si="2"/>
-        <v>33.28</v>
+        <v>33</v>
       </c>
       <c r="T13">
         <f t="shared" si="3"/>
@@ -3732,15 +3732,15 @@
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
-        <v>8.0000000000000004E-4</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="R14">
         <f t="shared" si="1"/>
-        <v>3.2000000000000002E-3</v>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="S14">
         <f t="shared" si="2"/>
-        <v>25.6</v>
+        <v>26</v>
       </c>
       <c r="T14">
         <f t="shared" si="3"/>
@@ -3793,15 +3793,15 @@
       </c>
       <c r="Q15">
         <f t="shared" si="0"/>
-        <v>8.0000000000000004E-4</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="R15">
         <f t="shared" si="1"/>
-        <v>3.2000000000000002E-3</v>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="S15">
         <f t="shared" si="2"/>
-        <v>25.6</v>
+        <v>26</v>
       </c>
       <c r="T15">
         <f t="shared" si="3"/>
@@ -3851,15 +3851,15 @@
       </c>
       <c r="Q16">
         <f t="shared" si="0"/>
-        <v>3.0999999999999999E-3</v>
+        <v>6.1999999999999998E-3</v>
       </c>
       <c r="R16">
         <f t="shared" si="1"/>
-        <v>1.24E-2</v>
+        <v>2.4799999999999999E-2</v>
       </c>
       <c r="S16">
         <f t="shared" si="2"/>
-        <v>44.8</v>
+        <v>45</v>
       </c>
       <c r="T16">
         <f t="shared" si="3"/>
@@ -3909,15 +3909,15 @@
       </c>
       <c r="Q17">
         <f t="shared" si="0"/>
-        <v>3.0999999999999999E-3</v>
+        <v>6.1999999999999998E-3</v>
       </c>
       <c r="R17">
         <f t="shared" si="1"/>
-        <v>1.24E-2</v>
+        <v>2.4799999999999999E-2</v>
       </c>
       <c r="S17">
         <f t="shared" si="2"/>
-        <v>38.4</v>
+        <v>38</v>
       </c>
       <c r="T17">
         <f t="shared" si="3"/>
@@ -3970,15 +3970,15 @@
       </c>
       <c r="Q18">
         <f t="shared" si="0"/>
-        <v>3.0999999999999999E-3</v>
+        <v>6.1999999999999998E-3</v>
       </c>
       <c r="R18">
         <f t="shared" si="1"/>
-        <v>1.24E-2</v>
+        <v>2.4799999999999999E-2</v>
       </c>
       <c r="S18">
         <f t="shared" si="2"/>
-        <v>44.8</v>
+        <v>45</v>
       </c>
       <c r="T18">
         <f t="shared" si="3"/>
@@ -4027,16 +4027,16 @@
         <v>246</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="0"/>
-        <v>8.9499999999999996E-3</v>
+        <f>E19/5000</f>
+        <v>1.7899999999999999E-2</v>
       </c>
       <c r="R19">
         <f t="shared" si="1"/>
-        <v>3.5799999999999998E-2</v>
+        <v>7.1599999999999997E-2</v>
       </c>
       <c r="S19">
         <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T19">
         <f t="shared" si="3"/>
@@ -4085,16 +4085,16 @@
         <v>246</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="0"/>
-        <v>7.1000000000000004E-3</v>
+        <f t="shared" ref="Q20:Q83" si="5">E20/5000</f>
+        <v>1.4200000000000001E-2</v>
       </c>
       <c r="R20">
         <f t="shared" si="1"/>
-        <v>2.8400000000000002E-2</v>
+        <v>5.6800000000000003E-2</v>
       </c>
       <c r="S20">
         <f t="shared" si="2"/>
-        <v>60.8</v>
+        <v>61</v>
       </c>
       <c r="T20">
         <f t="shared" si="3"/>
@@ -4143,16 +4143,16 @@
         <v>246</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="0"/>
-        <v>6.1000000000000004E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.2200000000000001E-2</v>
       </c>
       <c r="R21">
         <f t="shared" si="1"/>
-        <v>2.4400000000000002E-2</v>
+        <v>4.8800000000000003E-2</v>
       </c>
       <c r="S21">
         <f t="shared" si="2"/>
-        <v>52.48</v>
+        <v>52</v>
       </c>
       <c r="T21">
         <f t="shared" si="3"/>
@@ -4201,12 +4201,12 @@
         <v>246</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="0"/>
-        <v>4.1999999999999997E-3</v>
+        <f t="shared" si="5"/>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="R22">
         <f t="shared" si="1"/>
-        <v>1.6799999999999999E-2</v>
+        <v>3.3599999999999998E-2</v>
       </c>
       <c r="S22">
         <f t="shared" si="2"/>
@@ -4259,16 +4259,16 @@
         <v>246</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="0"/>
-        <v>2.8500000000000001E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="R23">
         <f t="shared" si="1"/>
-        <v>1.14E-2</v>
+        <v>2.2800000000000001E-2</v>
       </c>
       <c r="S23">
         <f t="shared" si="2"/>
-        <v>43.52</v>
+        <v>44</v>
       </c>
       <c r="T23">
         <f t="shared" si="3"/>
@@ -4317,16 +4317,16 @@
         <v>246</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="0"/>
-        <v>2.9499999999999999E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.8999999999999999E-3</v>
       </c>
       <c r="R24">
         <f t="shared" si="1"/>
-        <v>1.18E-2</v>
+        <v>2.3599999999999999E-2</v>
       </c>
       <c r="S24">
         <f t="shared" si="2"/>
-        <v>60.8</v>
+        <v>61</v>
       </c>
       <c r="T24">
         <f t="shared" si="3"/>
@@ -4375,16 +4375,16 @@
         <v>246</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="0"/>
-        <v>1.6000000000000001E-3</v>
+        <f t="shared" si="5"/>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="R25">
         <f t="shared" si="1"/>
-        <v>6.4000000000000003E-3</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="S25">
         <f t="shared" si="2"/>
-        <v>38.4</v>
+        <v>38</v>
       </c>
       <c r="T25">
         <f t="shared" si="3"/>
@@ -4433,16 +4433,16 @@
         <v>246</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="0"/>
-        <v>8.9999999999999998E-4</v>
+        <f t="shared" si="5"/>
+        <v>1.8E-3</v>
       </c>
       <c r="R26">
         <f t="shared" si="1"/>
-        <v>3.5999999999999999E-3</v>
+        <v>7.1999999999999998E-3</v>
       </c>
       <c r="S26">
         <f t="shared" si="2"/>
-        <v>28.8</v>
+        <v>29</v>
       </c>
       <c r="T26">
         <f t="shared" si="3"/>
@@ -4491,16 +4491,16 @@
         <v>246</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="0"/>
-        <v>2.0000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="R27">
         <f t="shared" si="1"/>
-        <v>8.0000000000000004E-4</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="S27">
         <f t="shared" si="2"/>
-        <v>22.4</v>
+        <v>22</v>
       </c>
       <c r="T27">
         <f t="shared" si="3"/>
@@ -4546,16 +4546,16 @@
         <v>246</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="0"/>
-        <v>3.0000000000000001E-3</v>
+        <f t="shared" si="5"/>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="R28">
         <f t="shared" si="1"/>
-        <v>1.2E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="S28">
         <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T28">
         <f t="shared" si="3"/>
@@ -4601,16 +4601,16 @@
         <v>246</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="0"/>
-        <v>2.2499999999999998E-3</v>
+        <f t="shared" si="5"/>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="R29">
         <f t="shared" si="1"/>
-        <v>8.9999999999999993E-3</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="S29">
         <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T29">
         <f t="shared" si="3"/>
@@ -4656,16 +4656,16 @@
         <v>246</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="0"/>
-        <v>1.75E-3</v>
+        <f t="shared" si="5"/>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="R30">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-3</v>
+        <v>1.4E-2</v>
       </c>
       <c r="S30">
         <f t="shared" si="2"/>
-        <v>60.8</v>
+        <v>61</v>
       </c>
       <c r="T30">
         <f t="shared" si="3"/>
@@ -4714,16 +4714,16 @@
         <v>246</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="0"/>
-        <v>1.4E-3</v>
+        <f t="shared" si="5"/>
+        <v>2.8E-3</v>
       </c>
       <c r="R31">
         <f t="shared" si="1"/>
-        <v>5.5999999999999999E-3</v>
+        <v>1.12E-2</v>
       </c>
       <c r="S31">
         <f t="shared" si="2"/>
-        <v>58.88</v>
+        <v>59</v>
       </c>
       <c r="T31">
         <f t="shared" si="3"/>
@@ -4775,18 +4775,18 @@
         <v>279</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001E-3</v>
+        <f t="shared" si="5"/>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="R32">
         <f t="shared" si="1"/>
-        <v>4.4000000000000003E-3</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="S32">
         <f t="shared" si="2"/>
-        <v>54.4</v>
-      </c>
-      <c r="T32">
+        <v>54</v>
+      </c>
+      <c r="T32" s="11">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -4833,16 +4833,16 @@
         <v>246</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="0"/>
-        <v>8.9999999999999998E-4</v>
+        <f t="shared" si="5"/>
+        <v>1.8E-3</v>
       </c>
       <c r="R33">
         <f t="shared" si="1"/>
-        <v>3.5999999999999999E-3</v>
+        <v>7.1999999999999998E-3</v>
       </c>
       <c r="S33">
         <f t="shared" si="2"/>
-        <v>52.48</v>
+        <v>52</v>
       </c>
       <c r="T33">
         <f t="shared" si="3"/>
@@ -4891,16 +4891,16 @@
         <v>246</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="0"/>
-        <v>5.5000000000000003E-4</v>
+        <f t="shared" si="5"/>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="R34">
         <f t="shared" si="1"/>
-        <v>2.2000000000000001E-3</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="S34">
         <f t="shared" si="2"/>
-        <v>44.8</v>
+        <v>45</v>
       </c>
       <c r="T34">
         <f t="shared" si="3"/>
@@ -4949,16 +4949,16 @@
         <v>246</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="0"/>
-        <v>2.9999999999999997E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="R35">
-        <f t="shared" si="1"/>
-        <v>1.1999999999999999E-3</v>
+        <f>Q35*4</f>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="S35">
         <f t="shared" si="2"/>
-        <v>38.4</v>
+        <v>38</v>
       </c>
       <c r="T35">
         <f t="shared" si="3"/>
@@ -5007,12 +5007,12 @@
         <v>246</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="0"/>
-        <v>1.4999999999999999E-4</v>
+        <f t="shared" si="5"/>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="R36">
         <f t="shared" si="1"/>
-        <v>5.9999999999999995E-4</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="S36">
         <f t="shared" si="2"/>
@@ -5065,16 +5065,16 @@
         <v>246</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="0"/>
-        <v>2.0000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="R37">
         <f t="shared" si="1"/>
-        <v>8.0000000000000004E-4</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="S37">
         <f t="shared" si="2"/>
-        <v>25.6</v>
+        <v>26</v>
       </c>
       <c r="T37">
         <f t="shared" si="3"/>
@@ -5123,16 +5123,16 @@
         <v>246</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="0"/>
-        <v>1E-4</v>
+        <f t="shared" si="5"/>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="R38">
         <f t="shared" si="1"/>
-        <v>4.0000000000000002E-4</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="S38">
         <f t="shared" si="2"/>
-        <v>21.12</v>
+        <v>21</v>
       </c>
       <c r="T38">
         <f t="shared" si="3"/>
@@ -5181,16 +5181,16 @@
         <v>246</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="0"/>
-        <v>1E-4</v>
+        <f t="shared" si="5"/>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="R39">
         <f t="shared" si="1"/>
-        <v>4.0000000000000002E-4</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="S39">
         <f t="shared" si="2"/>
-        <v>21.12</v>
+        <v>21</v>
       </c>
       <c r="T39">
         <f t="shared" si="3"/>
@@ -5239,15 +5239,15 @@
         <v>246</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="0"/>
-        <v>6.3499999999999997E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="R40">
         <f t="shared" si="1"/>
-        <v>2.5399999999999999E-2</v>
+        <v>5.0799999999999998E-2</v>
       </c>
       <c r="S40">
-        <f>120*B40/100</f>
+        <f>ROUND(120*B40/100,0)</f>
         <v>84</v>
       </c>
       <c r="T40">
@@ -5297,15 +5297,15 @@
         <v>246</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="0"/>
-        <v>5.2500000000000003E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="R41">
         <f t="shared" si="1"/>
-        <v>2.1000000000000001E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="S41">
-        <f t="shared" ref="S41:S51" si="5">120*B41/100</f>
+        <f t="shared" ref="S41:S54" si="6">ROUND(120*B41/100,0)</f>
         <v>132</v>
       </c>
       <c r="T41">
@@ -5355,15 +5355,15 @@
         <v>246</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="0"/>
-        <v>4.1000000000000003E-3</v>
+        <f t="shared" si="5"/>
+        <v>8.2000000000000007E-3</v>
       </c>
       <c r="R42">
         <f t="shared" si="1"/>
-        <v>1.6400000000000001E-2</v>
+        <v>3.2800000000000003E-2</v>
       </c>
       <c r="S42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>132</v>
       </c>
       <c r="T42">
@@ -5413,15 +5413,15 @@
         <v>246</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="R43">
         <f t="shared" si="1"/>
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="S43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>132</v>
       </c>
       <c r="T43">
@@ -5471,15 +5471,15 @@
         <v>246</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="0"/>
-        <v>1.9E-3</v>
+        <f t="shared" si="5"/>
+        <v>3.8E-3</v>
       </c>
       <c r="R44">
         <f t="shared" si="1"/>
-        <v>7.6E-3</v>
+        <v>1.52E-2</v>
       </c>
       <c r="S44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>132</v>
       </c>
       <c r="T44">
@@ -5529,15 +5529,15 @@
         <v>246</v>
       </c>
       <c r="Q45">
-        <f t="shared" si="0"/>
-        <v>1.4499999999999999E-3</v>
+        <f t="shared" si="5"/>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="R45">
         <f t="shared" si="1"/>
-        <v>5.7999999999999996E-3</v>
+        <v>1.1599999999999999E-2</v>
       </c>
       <c r="S45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>132</v>
       </c>
       <c r="T45">
@@ -5587,15 +5587,15 @@
         <v>246</v>
       </c>
       <c r="Q46">
-        <f t="shared" si="0"/>
-        <v>1E-3</v>
+        <f t="shared" si="5"/>
+        <v>2E-3</v>
       </c>
       <c r="R46">
         <f t="shared" si="1"/>
-        <v>4.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="S46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>132</v>
       </c>
       <c r="T46">
@@ -5645,15 +5645,15 @@
         <v>246</v>
       </c>
       <c r="Q47">
-        <f t="shared" si="0"/>
-        <v>5.9999999999999995E-4</v>
+        <f t="shared" si="5"/>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="R47">
         <f t="shared" si="1"/>
-        <v>2.3999999999999998E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="S47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>132</v>
       </c>
       <c r="T47">
@@ -5703,15 +5703,15 @@
         <v>246</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="0"/>
-        <v>5.9999999999999995E-4</v>
+        <f t="shared" si="5"/>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="R48">
         <f t="shared" si="1"/>
-        <v>2.3999999999999998E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="S48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>132</v>
       </c>
       <c r="T48">
@@ -5761,15 +5761,15 @@
         <v>246</v>
       </c>
       <c r="Q49">
-        <f t="shared" si="0"/>
-        <v>5.9999999999999995E-4</v>
+        <f t="shared" si="5"/>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="R49">
         <f t="shared" si="1"/>
-        <v>2.3999999999999998E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="S49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>132</v>
       </c>
       <c r="T49">
@@ -5819,15 +5819,15 @@
         <v>246</v>
       </c>
       <c r="Q50">
-        <f t="shared" si="0"/>
-        <v>4.0000000000000002E-4</v>
+        <f t="shared" si="5"/>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="R50">
         <f t="shared" si="1"/>
-        <v>1.6000000000000001E-3</v>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="S50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="T50">
@@ -5877,15 +5877,15 @@
         <v>246</v>
       </c>
       <c r="Q51">
-        <f t="shared" si="0"/>
-        <v>1E-4</v>
+        <f t="shared" si="5"/>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="R51">
         <f t="shared" si="1"/>
-        <v>4.0000000000000002E-4</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="S51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>72</v>
       </c>
       <c r="T51">
@@ -5935,16 +5935,16 @@
         <v>245</v>
       </c>
       <c r="Q52">
-        <f t="shared" si="0"/>
-        <v>3.4499999999999999E-3</v>
+        <f t="shared" si="5"/>
+        <v>6.8999999999999999E-3</v>
       </c>
       <c r="R52">
         <f t="shared" si="1"/>
-        <v>1.38E-2</v>
+        <v>2.76E-2</v>
       </c>
       <c r="S52">
-        <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <f t="shared" si="6"/>
+        <v>132</v>
       </c>
       <c r="T52">
         <f t="shared" si="3"/>
@@ -5993,16 +5993,16 @@
         <v>245</v>
       </c>
       <c r="Q53">
-        <f t="shared" si="0"/>
-        <v>2.3E-3</v>
+        <f t="shared" si="5"/>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="R53">
         <f t="shared" si="1"/>
-        <v>9.1999999999999998E-3</v>
+        <v>1.84E-2</v>
       </c>
       <c r="S53">
-        <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <f t="shared" si="6"/>
+        <v>132</v>
       </c>
       <c r="T53">
         <f t="shared" si="3"/>
@@ -6051,16 +6051,16 @@
         <v>245</v>
       </c>
       <c r="Q54">
-        <f t="shared" si="0"/>
-        <v>8.9999999999999998E-4</v>
+        <f t="shared" si="5"/>
+        <v>1.8E-3</v>
       </c>
       <c r="R54">
         <f t="shared" si="1"/>
-        <v>3.5999999999999999E-3</v>
+        <v>7.1999999999999998E-3</v>
       </c>
       <c r="S54">
-        <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <f t="shared" si="6"/>
+        <v>132</v>
       </c>
       <c r="T54">
         <f t="shared" si="3"/>
@@ -6109,16 +6109,16 @@
         <v>246</v>
       </c>
       <c r="Q55">
-        <f t="shared" si="0"/>
-        <v>1.65E-3</v>
+        <f t="shared" si="5"/>
+        <v>3.3E-3</v>
       </c>
       <c r="R55">
         <f t="shared" si="1"/>
-        <v>6.6E-3</v>
+        <v>1.32E-2</v>
       </c>
       <c r="S55">
         <f t="shared" si="2"/>
-        <v>57.6</v>
+        <v>58</v>
       </c>
       <c r="T55">
         <f t="shared" si="3"/>
@@ -6167,16 +6167,16 @@
         <v>246</v>
       </c>
       <c r="Q56">
-        <f t="shared" si="0"/>
-        <v>8.0000000000000004E-4</v>
+        <f t="shared" si="5"/>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="R56">
         <f t="shared" si="1"/>
-        <v>3.2000000000000002E-3</v>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="S56">
         <f t="shared" si="2"/>
-        <v>21.12</v>
+        <v>21</v>
       </c>
       <c r="T56">
         <f t="shared" si="3"/>
@@ -6225,16 +6225,16 @@
         <v>246</v>
       </c>
       <c r="Q57">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R57">
         <f t="shared" si="1"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S57">
         <f t="shared" si="2"/>
-        <v>60.8</v>
+        <v>61</v>
       </c>
       <c r="T57">
         <f t="shared" si="3"/>
@@ -6274,16 +6274,16 @@
         <v>245</v>
       </c>
       <c r="Q58">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R58">
         <f t="shared" si="1"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S58">
         <f t="shared" si="2"/>
-        <v>25.6</v>
+        <v>26</v>
       </c>
       <c r="T58">
         <f t="shared" si="3"/>
@@ -6304,7 +6304,7 @@
         <v>3</v>
       </c>
       <c r="E59">
-        <f t="shared" ref="E59:E77" si="6">AVERAGE(C59,D59)</f>
+        <f t="shared" ref="E59:E77" si="7">AVERAGE(C59,D59)</f>
         <v>2.5</v>
       </c>
       <c r="F59">
@@ -6323,16 +6323,16 @@
         <v>245</v>
       </c>
       <c r="Q59">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R59">
         <f t="shared" si="1"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S59">
         <f t="shared" si="2"/>
-        <v>23.04</v>
+        <v>23</v>
       </c>
       <c r="T59">
         <f t="shared" si="3"/>
@@ -6353,7 +6353,7 @@
         <v>3</v>
       </c>
       <c r="E60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="F60">
@@ -6378,16 +6378,16 @@
         <v>284</v>
       </c>
       <c r="Q60">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R60">
         <f t="shared" si="1"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S60">
         <f t="shared" si="2"/>
-        <v>51.2</v>
+        <v>51</v>
       </c>
       <c r="T60">
         <f t="shared" si="3"/>
@@ -6408,7 +6408,7 @@
         <v>3</v>
       </c>
       <c r="E61">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="F61">
@@ -6433,16 +6433,16 @@
         <v>284</v>
       </c>
       <c r="Q61">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R61">
         <f t="shared" si="1"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S61">
         <f t="shared" si="2"/>
-        <v>37.119999999999997</v>
+        <v>37</v>
       </c>
       <c r="T61">
         <f t="shared" si="3"/>
@@ -6463,7 +6463,7 @@
         <v>3</v>
       </c>
       <c r="E62">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="F62">
@@ -6482,16 +6482,16 @@
         <v>245</v>
       </c>
       <c r="Q62">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R62">
         <f t="shared" si="1"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S62">
         <f t="shared" si="2"/>
-        <v>38.4</v>
+        <v>38</v>
       </c>
       <c r="T62">
         <f t="shared" si="3"/>
@@ -6512,7 +6512,7 @@
         <v>3</v>
       </c>
       <c r="E63">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="F63">
@@ -6531,16 +6531,16 @@
         <v>245</v>
       </c>
       <c r="Q63">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R63">
         <f t="shared" si="1"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S63">
         <f t="shared" si="2"/>
-        <v>50.56</v>
+        <v>51</v>
       </c>
       <c r="T63">
         <f t="shared" si="3"/>
@@ -6561,7 +6561,7 @@
         <v>3</v>
       </c>
       <c r="E64">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="F64">
@@ -6586,16 +6586,16 @@
         <v>284</v>
       </c>
       <c r="Q64">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R64">
         <f t="shared" si="1"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S64">
         <f t="shared" si="2"/>
-        <v>32.64</v>
+        <v>33</v>
       </c>
       <c r="T64">
         <f t="shared" si="3"/>
@@ -6616,7 +6616,7 @@
         <v>3</v>
       </c>
       <c r="E65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="F65">
@@ -6641,16 +6641,16 @@
         <v>284</v>
       </c>
       <c r="Q65">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R65">
         <f t="shared" si="1"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S65">
         <f t="shared" si="2"/>
-        <v>42.88</v>
+        <v>43</v>
       </c>
       <c r="T65">
         <f t="shared" si="3"/>
@@ -6671,7 +6671,7 @@
         <v>3</v>
       </c>
       <c r="E66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="F66">
@@ -6696,16 +6696,16 @@
         <v>246</v>
       </c>
       <c r="Q66">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R66">
         <f t="shared" si="1"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S66">
         <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T66">
         <f t="shared" si="3"/>
@@ -6726,7 +6726,7 @@
         <v>3</v>
       </c>
       <c r="E67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="F67">
@@ -6751,16 +6751,16 @@
         <v>284</v>
       </c>
       <c r="Q67">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R67">
         <f t="shared" si="1"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S67">
         <f t="shared" si="2"/>
-        <v>33.92</v>
+        <v>34</v>
       </c>
       <c r="T67">
         <f t="shared" si="3"/>
@@ -6781,7 +6781,7 @@
         <v>84</v>
       </c>
       <c r="E68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76</v>
       </c>
       <c r="F68">
@@ -6806,16 +6806,16 @@
         <v>246</v>
       </c>
       <c r="Q68">
-        <f t="shared" si="0"/>
-        <v>7.6E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.52E-2</v>
       </c>
       <c r="R68">
-        <f t="shared" si="1"/>
-        <v>3.04E-2</v>
+        <f t="shared" ref="R68:R98" si="8">Q68*4</f>
+        <v>6.08E-2</v>
       </c>
       <c r="S68">
         <f t="shared" si="2"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T68">
         <f t="shared" si="3"/>
@@ -6836,7 +6836,7 @@
         <v>3</v>
       </c>
       <c r="E69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="F69">
@@ -6861,16 +6861,16 @@
         <v>284</v>
       </c>
       <c r="Q69">
-        <f t="shared" ref="Q69:Q98" si="7">E69/10000</f>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R69">
-        <f t="shared" ref="R69:R98" si="8">E69/2500</f>
-        <v>1E-3</v>
+        <f t="shared" si="8"/>
+        <v>2E-3</v>
       </c>
       <c r="S69">
-        <f t="shared" ref="S69:S98" si="9">64*B69/100</f>
-        <v>62.08</v>
+        <f t="shared" ref="S69:S98" si="9">ROUND(64*B69/100,0)</f>
+        <v>62</v>
       </c>
       <c r="T69">
         <f t="shared" ref="T69:T98" si="10">ROUNDUP(E69/15,0)</f>
@@ -6891,7 +6891,7 @@
         <v>3</v>
       </c>
       <c r="E70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="F70">
@@ -6910,16 +6910,16 @@
         <v>245</v>
       </c>
       <c r="Q70">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R70">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S70">
         <f t="shared" si="9"/>
-        <v>26.24</v>
+        <v>26</v>
       </c>
       <c r="T70">
         <f t="shared" si="10"/>
@@ -6940,7 +6940,7 @@
         <v>3</v>
       </c>
       <c r="E71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="F71">
@@ -6965,16 +6965,16 @@
         <v>284</v>
       </c>
       <c r="Q71">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R71">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S71">
         <f t="shared" si="9"/>
-        <v>55.04</v>
+        <v>55</v>
       </c>
       <c r="T71">
         <f t="shared" si="10"/>
@@ -6995,7 +6995,7 @@
         <v>84</v>
       </c>
       <c r="E72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76</v>
       </c>
       <c r="F72">
@@ -7020,16 +7020,16 @@
         <v>246</v>
       </c>
       <c r="Q72">
-        <f t="shared" si="7"/>
-        <v>7.6E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.52E-2</v>
       </c>
       <c r="R72">
         <f t="shared" si="8"/>
-        <v>3.04E-2</v>
+        <v>6.08E-2</v>
       </c>
       <c r="S72">
         <f t="shared" si="9"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T72">
         <f t="shared" si="10"/>
@@ -7050,7 +7050,7 @@
         <v>2</v>
       </c>
       <c r="E73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="F73">
@@ -7075,16 +7075,16 @@
         <v>246</v>
       </c>
       <c r="Q73">
-        <f t="shared" si="7"/>
-        <v>1E-4</v>
+        <f t="shared" si="5"/>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="R73">
         <f t="shared" si="8"/>
-        <v>4.0000000000000002E-4</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="S73">
         <f t="shared" si="9"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T73">
         <f t="shared" si="10"/>
@@ -7105,7 +7105,7 @@
         <v>3</v>
       </c>
       <c r="E74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="F74">
@@ -7136,16 +7136,16 @@
         <v>284</v>
       </c>
       <c r="Q74">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R74">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S74">
         <f t="shared" si="9"/>
-        <v>46.08</v>
+        <v>46</v>
       </c>
       <c r="T74">
         <f t="shared" si="10"/>
@@ -7166,7 +7166,7 @@
         <v>84</v>
       </c>
       <c r="E75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76</v>
       </c>
       <c r="F75">
@@ -7191,16 +7191,16 @@
         <v>246</v>
       </c>
       <c r="Q75">
-        <f t="shared" si="7"/>
-        <v>7.6E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.52E-2</v>
       </c>
       <c r="R75">
         <f t="shared" si="8"/>
-        <v>3.04E-2</v>
+        <v>6.08E-2</v>
       </c>
       <c r="S75">
         <f t="shared" si="9"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T75">
         <f t="shared" si="10"/>
@@ -7221,7 +7221,7 @@
         <v>3</v>
       </c>
       <c r="E76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
       <c r="F76">
@@ -7246,16 +7246,16 @@
         <v>246</v>
       </c>
       <c r="Q76">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R76">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S76">
         <f t="shared" si="9"/>
-        <v>19.2</v>
+        <v>19</v>
       </c>
       <c r="T76">
         <f t="shared" si="10"/>
@@ -7276,7 +7276,7 @@
         <v>38</v>
       </c>
       <c r="E77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>37</v>
       </c>
       <c r="F77">
@@ -7307,16 +7307,16 @@
         <v>285</v>
       </c>
       <c r="Q77">
-        <f t="shared" si="7"/>
-        <v>3.7000000000000002E-3</v>
+        <f t="shared" si="5"/>
+        <v>7.4000000000000003E-3</v>
       </c>
       <c r="R77">
         <f t="shared" si="8"/>
-        <v>1.4800000000000001E-2</v>
+        <v>2.9600000000000001E-2</v>
       </c>
       <c r="S77">
         <f t="shared" si="9"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T77">
         <f t="shared" si="10"/>
@@ -7365,16 +7365,16 @@
         <v>298</v>
       </c>
       <c r="Q78">
-        <f t="shared" si="7"/>
-        <v>3.15E-3</v>
+        <f t="shared" si="5"/>
+        <v>6.3E-3</v>
       </c>
       <c r="R78">
         <f t="shared" si="8"/>
-        <v>1.26E-2</v>
+        <v>2.52E-2</v>
       </c>
       <c r="S78">
         <f t="shared" si="9"/>
-        <v>45.44</v>
+        <v>45</v>
       </c>
       <c r="T78">
         <f t="shared" si="10"/>
@@ -7414,16 +7414,16 @@
         <v>245</v>
       </c>
       <c r="Q79">
-        <f t="shared" si="7"/>
-        <v>6.2500000000000003E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="R79">
         <f t="shared" si="8"/>
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="S79">
         <f t="shared" si="9"/>
-        <v>62.08</v>
+        <v>62</v>
       </c>
       <c r="T79">
         <f t="shared" si="10"/>
@@ -7469,16 +7469,16 @@
         <v>246</v>
       </c>
       <c r="Q80">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R80">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S80">
         <f t="shared" si="9"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T80">
         <f t="shared" si="10"/>
@@ -7524,16 +7524,16 @@
         <v>286</v>
       </c>
       <c r="Q81">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R81">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S81">
         <f t="shared" si="9"/>
-        <v>50.56</v>
+        <v>51</v>
       </c>
       <c r="T81">
         <f t="shared" si="10"/>
@@ -7573,16 +7573,16 @@
         <v>245</v>
       </c>
       <c r="Q82">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R82">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S82">
         <f t="shared" si="9"/>
-        <v>62.08</v>
+        <v>62</v>
       </c>
       <c r="T82">
         <f t="shared" si="10"/>
@@ -7622,16 +7622,16 @@
         <v>245</v>
       </c>
       <c r="Q83">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R83">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S83">
         <f t="shared" si="9"/>
-        <v>53.76</v>
+        <v>54</v>
       </c>
       <c r="T83">
         <f t="shared" si="10"/>
@@ -7671,12 +7671,12 @@
         <v>245</v>
       </c>
       <c r="Q84">
-        <f t="shared" si="7"/>
-        <v>5.0000000000000002E-5</v>
+        <f t="shared" ref="Q84:Q98" si="12">E84/5000</f>
+        <v>1E-4</v>
       </c>
       <c r="R84">
         <f t="shared" si="8"/>
-        <v>2.0000000000000001E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="S84">
         <f t="shared" si="9"/>
@@ -7726,16 +7726,16 @@
         <v>246</v>
       </c>
       <c r="Q85">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="12"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R85">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S85">
         <f t="shared" si="9"/>
-        <v>56.32</v>
+        <v>56</v>
       </c>
       <c r="T85">
         <f t="shared" si="10"/>
@@ -7781,16 +7781,16 @@
         <v>284</v>
       </c>
       <c r="Q86">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="12"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R86">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S86">
         <f t="shared" si="9"/>
-        <v>28.8</v>
+        <v>29</v>
       </c>
       <c r="T86">
         <f t="shared" si="10"/>
@@ -7830,16 +7830,16 @@
         <v>245</v>
       </c>
       <c r="Q87">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="12"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R87">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S87">
         <f t="shared" si="9"/>
-        <v>22.4</v>
+        <v>22</v>
       </c>
       <c r="T87">
         <f t="shared" si="10"/>
@@ -7860,7 +7860,7 @@
         <v>3</v>
       </c>
       <c r="E88">
-        <f t="shared" ref="E88:E94" si="12">AVERAGE(C88,D88)</f>
+        <f t="shared" ref="E88:E94" si="13">AVERAGE(C88,D88)</f>
         <v>2.5</v>
       </c>
       <c r="F88">
@@ -7891,16 +7891,16 @@
         <v>284</v>
       </c>
       <c r="Q88">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="12"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R88">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S88">
         <f t="shared" si="9"/>
-        <v>40.96</v>
+        <v>41</v>
       </c>
       <c r="T88">
         <f t="shared" si="10"/>
@@ -7921,7 +7921,7 @@
         <v>3</v>
       </c>
       <c r="E89">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.5</v>
       </c>
       <c r="F89">
@@ -7946,16 +7946,16 @@
         <v>246</v>
       </c>
       <c r="Q89">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="12"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R89">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S89">
         <f t="shared" si="9"/>
-        <v>70.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="T89">
         <f t="shared" si="10"/>
@@ -7976,7 +7976,7 @@
         <v>3</v>
       </c>
       <c r="E90">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.5</v>
       </c>
       <c r="F90">
@@ -8007,16 +8007,16 @@
         <v>284</v>
       </c>
       <c r="Q90">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="12"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R90">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S90">
         <f t="shared" si="9"/>
-        <v>26.88</v>
+        <v>27</v>
       </c>
       <c r="T90">
         <f t="shared" si="10"/>
@@ -8037,7 +8037,7 @@
         <v>3</v>
       </c>
       <c r="E91">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.5</v>
       </c>
       <c r="F91">
@@ -8068,16 +8068,16 @@
         <v>286</v>
       </c>
       <c r="Q91">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="12"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R91">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S91">
         <f t="shared" si="9"/>
-        <v>62.08</v>
+        <v>62</v>
       </c>
       <c r="T91">
         <f t="shared" si="10"/>
@@ -8098,7 +8098,7 @@
         <v>12</v>
       </c>
       <c r="E92">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="F92">
@@ -8123,16 +8123,16 @@
         <v>246</v>
       </c>
       <c r="Q92">
-        <f t="shared" si="7"/>
-        <v>8.0000000000000004E-4</v>
+        <f t="shared" si="12"/>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="R92">
         <f t="shared" si="8"/>
-        <v>3.2000000000000002E-3</v>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="S92">
         <f t="shared" si="9"/>
-        <v>21.12</v>
+        <v>21</v>
       </c>
       <c r="T92">
         <f t="shared" si="10"/>
@@ -8153,7 +8153,7 @@
         <v>3</v>
       </c>
       <c r="E93">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.5</v>
       </c>
       <c r="F93">
@@ -8178,16 +8178,16 @@
         <v>245</v>
       </c>
       <c r="Q93">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="12"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R93">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S93">
         <f t="shared" si="9"/>
-        <v>40.32</v>
+        <v>40</v>
       </c>
       <c r="T93">
         <f t="shared" si="10"/>
@@ -8208,7 +8208,7 @@
         <v>3</v>
       </c>
       <c r="E94">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.5</v>
       </c>
       <c r="F94">
@@ -8233,16 +8233,16 @@
         <v>245</v>
       </c>
       <c r="Q94">
-        <f t="shared" si="7"/>
-        <v>2.5000000000000001E-4</v>
+        <f t="shared" si="12"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="R94">
         <f t="shared" si="8"/>
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="S94">
         <f t="shared" si="9"/>
-        <v>19.2</v>
+        <v>19</v>
       </c>
       <c r="T94">
         <f t="shared" si="10"/>
@@ -8291,16 +8291,16 @@
         <v>246</v>
       </c>
       <c r="Q95">
-        <f t="shared" si="7"/>
-        <v>6.9999999999999999E-4</v>
+        <f t="shared" si="12"/>
+        <v>1.4E-3</v>
       </c>
       <c r="R95">
         <f t="shared" si="8"/>
-        <v>2.8E-3</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="S95">
         <f t="shared" si="9"/>
-        <v>14.08</v>
+        <v>14</v>
       </c>
       <c r="T95">
         <f t="shared" si="10"/>
@@ -8349,16 +8349,16 @@
         <v>246</v>
       </c>
       <c r="Q96">
-        <f t="shared" si="7"/>
-        <v>6.9999999999999999E-4</v>
+        <f t="shared" si="12"/>
+        <v>1.4E-3</v>
       </c>
       <c r="R96">
         <f t="shared" si="8"/>
-        <v>2.8E-3</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="S96">
         <f t="shared" si="9"/>
-        <v>14.08</v>
+        <v>14</v>
       </c>
       <c r="T96">
         <f t="shared" si="10"/>
@@ -8407,16 +8407,16 @@
         <v>246</v>
       </c>
       <c r="Q97">
-        <f t="shared" si="7"/>
-        <v>6.9999999999999999E-4</v>
+        <f t="shared" si="12"/>
+        <v>1.4E-3</v>
       </c>
       <c r="R97">
         <f t="shared" si="8"/>
-        <v>2.8E-3</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="S97">
         <f t="shared" si="9"/>
-        <v>14.08</v>
+        <v>14</v>
       </c>
       <c r="T97">
         <f t="shared" si="10"/>
@@ -8465,16 +8465,16 @@
         <v>246</v>
       </c>
       <c r="Q98">
-        <f t="shared" si="7"/>
-        <v>6.9999999999999999E-4</v>
+        <f t="shared" si="12"/>
+        <v>1.4E-3</v>
       </c>
       <c r="R98">
         <f t="shared" si="8"/>
-        <v>2.8E-3</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="S98">
         <f t="shared" si="9"/>
-        <v>14.08</v>
+        <v>14</v>
       </c>
       <c r="T98">
         <f t="shared" si="10"/>

</xml_diff>